<commit_message>
Push demographic visual drafts to main
Push demographic visual drafts to main
</commit_message>
<xml_diff>
--- a/outside_data/PITS Chicago 2023 Data.xlsx
+++ b/outside_data/PITS Chicago 2023 Data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\higgi\Documents\GitHub\Housing-and-Migrants-Chicago\outside_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{235942EE-76A3-4FED-A621-A8420C98AE68}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C76A566-EFFB-46FD-96F5-31A67D03AB06}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="1" xr2:uid="{D489DE06-1593-463A-9161-497C05F1C863}"/>
+    <workbookView xWindow="-90" yWindow="0" windowWidth="9780" windowHeight="10170" firstSheet="6" activeTab="8" xr2:uid="{D489DE06-1593-463A-9161-497C05F1C863}"/>
   </bookViews>
   <sheets>
     <sheet name="Read Me" sheetId="3" r:id="rId1"/>
@@ -320,15 +320,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -647,7 +647,7 @@
   <dimension ref="A1:A10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+      <selection activeCell="A17" sqref="A17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -681,12 +681,12 @@
       </c>
     </row>
     <row r="7" spans="1:1" ht="29" x14ac:dyDescent="0.35">
-      <c r="A7" s="6" t="s">
+      <c r="A7" s="4" t="s">
         <v>70</v>
       </c>
     </row>
     <row r="8" spans="1:1" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A8" s="6" t="s">
+      <c r="A8" s="4" t="s">
         <v>69</v>
       </c>
     </row>
@@ -709,25 +709,25 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{05B9E380-2467-411D-A968-517B23B9FDCE}">
   <dimension ref="A1:G17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="I11" sqref="I11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="C1" s="3"/>
-      <c r="D1" s="3" t="s">
+      <c r="C1" s="5"/>
+      <c r="D1" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="E1" s="3"/>
-      <c r="F1" s="3" t="s">
+      <c r="E1" s="5"/>
+      <c r="F1" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="G1" s="3"/>
+      <c r="G1" s="5"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
@@ -1118,18 +1118,18 @@
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="C1" s="3"/>
-      <c r="D1" s="3" t="s">
+      <c r="C1" s="5"/>
+      <c r="D1" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="E1" s="3"/>
-      <c r="F1" s="3" t="s">
+      <c r="E1" s="5"/>
+      <c r="F1" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="G1" s="3"/>
+      <c r="G1" s="5"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
@@ -1161,7 +1161,7 @@
       <c r="B3">
         <v>555</v>
       </c>
-      <c r="C3" s="4">
+      <c r="C3" s="3">
         <v>0.77800000000000002</v>
       </c>
       <c r="D3">
@@ -1173,7 +1173,7 @@
       <c r="F3">
         <v>546</v>
       </c>
-      <c r="G3" s="4">
+      <c r="G3" s="3">
         <v>0.75</v>
       </c>
     </row>
@@ -1490,7 +1490,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{04C81B61-06B9-4567-AE23-24E23BAD5989}">
   <dimension ref="A1:Q17"/>
   <sheetViews>
-    <sheetView topLeftCell="A6" workbookViewId="0">
+    <sheetView topLeftCell="A5" workbookViewId="0">
       <selection activeCell="L16" sqref="L16"/>
     </sheetView>
   </sheetViews>
@@ -1556,37 +1556,37 @@
       <c r="A2" t="s">
         <v>14</v>
       </c>
-      <c r="B2" s="4">
+      <c r="B2" s="3">
         <v>0.32700000000000001</v>
       </c>
-      <c r="C2" s="4">
+      <c r="C2" s="3">
         <v>0.40400000000000003</v>
       </c>
-      <c r="D2" s="4">
+      <c r="D2" s="3">
         <v>0.45400000000000001</v>
       </c>
-      <c r="E2" s="4">
+      <c r="E2" s="3">
         <v>0.44700000000000001</v>
       </c>
-      <c r="F2" s="4">
+      <c r="F2" s="3">
         <v>0.45</v>
       </c>
-      <c r="G2" s="4">
+      <c r="G2" s="3">
         <v>0.41</v>
       </c>
-      <c r="H2" s="4">
+      <c r="H2" s="3">
         <v>0.42199999999999999</v>
       </c>
-      <c r="I2" s="4">
+      <c r="I2" s="3">
         <v>0.4</v>
       </c>
-      <c r="J2" s="4">
+      <c r="J2" s="3">
         <v>0.43099999999999999</v>
       </c>
-      <c r="K2" s="4">
+      <c r="K2" s="3">
         <v>0.42099999999999999</v>
       </c>
-      <c r="L2" s="4">
+      <c r="L2" s="3">
         <v>0.42699999999999999</v>
       </c>
       <c r="M2" s="2">
@@ -1609,37 +1609,37 @@
       <c r="A3" t="s">
         <v>13</v>
       </c>
-      <c r="B3" s="4">
+      <c r="B3" s="3">
         <v>0.66700000000000004</v>
       </c>
-      <c r="C3" s="4">
+      <c r="C3" s="3">
         <v>0.58599999999999997</v>
       </c>
-      <c r="D3" s="4">
+      <c r="D3" s="3">
         <v>0.54300000000000004</v>
       </c>
-      <c r="E3" s="4">
+      <c r="E3" s="3">
         <v>0.54800000000000004</v>
       </c>
-      <c r="F3" s="4">
+      <c r="F3" s="3">
         <v>0.54400000000000004</v>
       </c>
-      <c r="G3" s="4">
+      <c r="G3" s="3">
         <v>0.58099999999999996</v>
       </c>
-      <c r="H3" s="4">
+      <c r="H3" s="3">
         <v>0.57299999999999995</v>
       </c>
-      <c r="I3" s="4">
+      <c r="I3" s="3">
         <v>0.59499999999999997</v>
       </c>
-      <c r="J3" s="4">
+      <c r="J3" s="3">
         <v>0.56499999999999995</v>
       </c>
-      <c r="K3" s="4">
+      <c r="K3" s="3">
         <v>0.57899999999999996</v>
       </c>
-      <c r="L3" s="4">
+      <c r="L3" s="3">
         <v>0.57299999999999995</v>
       </c>
       <c r="M3" s="2">
@@ -1662,31 +1662,31 @@
       <c r="A4" t="s">
         <v>15</v>
       </c>
-      <c r="B4" s="4">
+      <c r="B4" s="3">
         <v>6.0000000000000001E-3</v>
       </c>
-      <c r="C4" s="4">
+      <c r="C4" s="3">
         <v>7.0000000000000001E-3</v>
       </c>
-      <c r="D4" s="4">
+      <c r="D4" s="3">
         <v>2E-3</v>
       </c>
-      <c r="E4" s="4">
+      <c r="E4" s="3">
         <v>4.0000000000000001E-3</v>
       </c>
-      <c r="F4" s="4">
+      <c r="F4" s="3">
         <v>5.0000000000000001E-3</v>
       </c>
-      <c r="G4" s="4">
+      <c r="G4" s="3">
         <v>5.0000000000000001E-3</v>
       </c>
-      <c r="H4" s="4">
+      <c r="H4" s="3">
         <v>3.0000000000000001E-3</v>
       </c>
-      <c r="I4" s="4">
+      <c r="I4" s="3">
         <v>5.0000000000000001E-3</v>
       </c>
-      <c r="J4" s="4">
+      <c r="J4" s="3">
         <v>5.0000000000000001E-3</v>
       </c>
       <c r="K4" t="s">
@@ -1715,22 +1715,22 @@
       <c r="A5" t="s">
         <v>16</v>
       </c>
-      <c r="B5" s="4">
+      <c r="B5" s="3">
         <v>2E-3</v>
       </c>
-      <c r="C5" s="4">
+      <c r="C5" s="3">
         <v>3.0000000000000001E-3</v>
       </c>
-      <c r="D5" s="4">
+      <c r="D5" s="3">
         <v>1E-3</v>
       </c>
-      <c r="E5" s="4">
+      <c r="E5" s="3">
         <v>1E-3</v>
       </c>
-      <c r="F5" s="4">
+      <c r="F5" s="3">
         <v>2E-3</v>
       </c>
-      <c r="G5" s="4">
+      <c r="G5" s="3">
         <v>4.0000000000000001E-3</v>
       </c>
       <c r="H5" t="s">
@@ -1765,12 +1765,12 @@
       </c>
     </row>
     <row r="6" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="B6" s="4"/>
-      <c r="C6" s="4"/>
-      <c r="D6" s="4"/>
-      <c r="E6" s="4"/>
-      <c r="F6" s="4"/>
-      <c r="G6" s="4"/>
+      <c r="B6" s="3"/>
+      <c r="C6" s="3"/>
+      <c r="D6" s="3"/>
+      <c r="E6" s="3"/>
+      <c r="F6" s="3"/>
+      <c r="G6" s="3"/>
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
@@ -1829,37 +1829,37 @@
       <c r="A8" t="s">
         <v>14</v>
       </c>
-      <c r="B8" s="4">
+      <c r="B8" s="3">
         <v>0.23100000000000001</v>
       </c>
-      <c r="C8" s="4">
+      <c r="C8" s="3">
         <v>0.14799999999999999</v>
       </c>
-      <c r="D8" s="4">
+      <c r="D8" s="3">
         <v>0.182</v>
       </c>
-      <c r="E8" s="4">
+      <c r="E8" s="3">
         <v>0.21299999999999999</v>
       </c>
-      <c r="F8" s="4">
+      <c r="F8" s="3">
         <v>0.19500000000000001</v>
       </c>
-      <c r="G8" s="4">
+      <c r="G8" s="3">
         <v>0.153</v>
       </c>
-      <c r="H8" s="4">
+      <c r="H8" s="3">
         <v>0.16800000000000001</v>
       </c>
-      <c r="I8" s="4">
+      <c r="I8" s="3">
         <v>0.16200000000000001</v>
       </c>
-      <c r="J8" s="4">
+      <c r="J8" s="3">
         <v>0.13200000000000001</v>
       </c>
-      <c r="K8" s="4">
+      <c r="K8" s="3">
         <v>0.18099999999999999</v>
       </c>
-      <c r="L8" s="4">
+      <c r="L8" s="3">
         <v>0.185</v>
       </c>
       <c r="M8" t="s">
@@ -1882,37 +1882,37 @@
       <c r="A9" t="s">
         <v>13</v>
       </c>
-      <c r="B9" s="4">
+      <c r="B9" s="3">
         <v>0.76800000000000002</v>
       </c>
-      <c r="C9" s="4">
+      <c r="C9" s="3">
         <v>0.84899999999999998</v>
       </c>
-      <c r="D9" s="4">
+      <c r="D9" s="3">
         <v>0.81799999999999995</v>
       </c>
-      <c r="E9" s="4">
+      <c r="E9" s="3">
         <v>0.78700000000000003</v>
       </c>
-      <c r="F9" s="4">
+      <c r="F9" s="3">
         <v>0.79700000000000004</v>
       </c>
-      <c r="G9" s="4">
+      <c r="G9" s="3">
         <v>0.84699999999999998</v>
       </c>
-      <c r="H9" s="4">
+      <c r="H9" s="3">
         <v>0.83199999999999996</v>
       </c>
-      <c r="I9" s="4">
+      <c r="I9" s="3">
         <v>0.83499999999999996</v>
       </c>
-      <c r="J9" s="4">
+      <c r="J9" s="3">
         <v>0.86699999999999999</v>
       </c>
-      <c r="K9" s="4">
+      <c r="K9" s="3">
         <v>0.81899999999999995</v>
       </c>
-      <c r="L9" s="4">
+      <c r="L9" s="3">
         <v>0.81499999999999995</v>
       </c>
       <c r="M9" t="s">
@@ -1935,31 +1935,31 @@
       <c r="A10" t="s">
         <v>15</v>
       </c>
-      <c r="B10" s="4">
-        <v>0</v>
-      </c>
-      <c r="C10" s="4">
+      <c r="B10" s="3">
+        <v>0</v>
+      </c>
+      <c r="C10" s="3">
         <v>3.0000000000000001E-3</v>
       </c>
-      <c r="D10" s="4">
-        <v>0</v>
-      </c>
-      <c r="E10" s="4">
-        <v>0</v>
-      </c>
-      <c r="F10" s="4">
+      <c r="D10" s="3">
+        <v>0</v>
+      </c>
+      <c r="E10" s="3">
+        <v>0</v>
+      </c>
+      <c r="F10" s="3">
         <v>6.0000000000000001E-3</v>
       </c>
-      <c r="G10" s="4">
-        <v>0</v>
-      </c>
-      <c r="H10" s="4">
+      <c r="G10" s="3">
+        <v>0</v>
+      </c>
+      <c r="H10" s="3">
         <v>1E-3</v>
       </c>
-      <c r="I10" s="4">
+      <c r="I10" s="3">
         <v>3.0000000000000001E-3</v>
       </c>
-      <c r="J10" s="4">
+      <c r="J10" s="3">
         <v>1E-3</v>
       </c>
       <c r="K10" t="s">
@@ -1988,22 +1988,22 @@
       <c r="A11" t="s">
         <v>16</v>
       </c>
-      <c r="B11" s="4">
+      <c r="B11" s="3">
         <v>1E-3</v>
       </c>
-      <c r="C11" s="4">
-        <v>0</v>
-      </c>
-      <c r="D11" s="4">
-        <v>0</v>
-      </c>
-      <c r="E11" s="4">
-        <v>0</v>
-      </c>
-      <c r="F11" s="4">
+      <c r="C11" s="3">
+        <v>0</v>
+      </c>
+      <c r="D11" s="3">
+        <v>0</v>
+      </c>
+      <c r="E11" s="3">
+        <v>0</v>
+      </c>
+      <c r="F11" s="3">
         <v>2E-3</v>
       </c>
-      <c r="G11" s="4">
+      <c r="G11" s="3">
         <v>0</v>
       </c>
       <c r="H11" t="s">
@@ -2094,37 +2094,37 @@
       <c r="A14" t="s">
         <v>14</v>
       </c>
-      <c r="B14" s="4">
+      <c r="B14" s="3">
         <v>0.68200000000000005</v>
       </c>
-      <c r="C14" s="4">
+      <c r="C14" s="3">
         <v>0.67200000000000004</v>
       </c>
-      <c r="D14" s="4">
+      <c r="D14" s="3">
         <v>0.59499999999999997</v>
       </c>
-      <c r="E14" s="4">
+      <c r="E14" s="3">
         <v>0.61599999999999999</v>
       </c>
-      <c r="F14" s="4">
+      <c r="F14" s="3">
         <v>0.61099999999999999</v>
       </c>
-      <c r="G14" s="4">
+      <c r="G14" s="3">
         <v>0.66600000000000004</v>
       </c>
-      <c r="H14" s="4">
+      <c r="H14" s="3">
         <v>0.66300000000000003</v>
       </c>
-      <c r="I14" s="4">
+      <c r="I14" s="3">
         <v>0.66</v>
       </c>
-      <c r="J14" s="4">
+      <c r="J14" s="3">
         <v>0.67900000000000005</v>
       </c>
-      <c r="K14" s="4">
+      <c r="K14" s="3">
         <v>0.628</v>
       </c>
-      <c r="L14" s="4">
+      <c r="L14" s="3">
         <v>0.63300000000000001</v>
       </c>
       <c r="M14" t="s">
@@ -2147,37 +2147,37 @@
       <c r="A15" t="s">
         <v>13</v>
       </c>
-      <c r="B15" s="4">
+      <c r="B15" s="3">
         <v>0.68200000000000005</v>
       </c>
-      <c r="C15" s="4">
+      <c r="C15" s="3">
         <v>0.67200000000000004</v>
       </c>
-      <c r="D15" s="4">
+      <c r="D15" s="3">
         <v>0.59499999999999997</v>
       </c>
-      <c r="E15" s="4">
+      <c r="E15" s="3">
         <v>0.61599999999999999</v>
       </c>
-      <c r="F15" s="4">
+      <c r="F15" s="3">
         <v>0.61099999999999999</v>
       </c>
-      <c r="G15" s="4">
+      <c r="G15" s="3">
         <v>0.66600000000000004</v>
       </c>
-      <c r="H15" s="4">
+      <c r="H15" s="3">
         <v>0.66300000000000003</v>
       </c>
-      <c r="I15" s="4">
+      <c r="I15" s="3">
         <v>0.66</v>
       </c>
-      <c r="J15" s="4">
+      <c r="J15" s="3">
         <v>0.67900000000000005</v>
       </c>
-      <c r="K15" s="4">
+      <c r="K15" s="3">
         <v>0.628</v>
       </c>
-      <c r="L15" s="4">
+      <c r="L15" s="3">
         <v>0.63300000000000001</v>
       </c>
       <c r="M15" t="s">
@@ -2200,22 +2200,22 @@
       <c r="A16" t="s">
         <v>15</v>
       </c>
-      <c r="B16" s="4">
+      <c r="B16" s="3">
         <v>2E-3</v>
       </c>
-      <c r="C16" s="4">
+      <c r="C16" s="3">
         <v>2E-3</v>
       </c>
-      <c r="D16" s="4">
+      <c r="D16" s="3">
         <v>1E-3</v>
       </c>
-      <c r="E16" s="4">
+      <c r="E16" s="3">
         <v>1E-3</v>
       </c>
-      <c r="F16" s="4">
+      <c r="F16" s="3">
         <v>2E-3</v>
       </c>
-      <c r="G16" s="4">
+      <c r="G16" s="3">
         <v>3.0000000000000001E-3</v>
       </c>
       <c r="H16" t="s">
@@ -2253,22 +2253,22 @@
       <c r="A17" t="s">
         <v>16</v>
       </c>
-      <c r="B17" s="4">
+      <c r="B17" s="3">
         <v>2E-3</v>
       </c>
-      <c r="C17" s="4">
+      <c r="C17" s="3">
         <v>2E-3</v>
       </c>
-      <c r="D17" s="4">
+      <c r="D17" s="3">
         <v>1E-3</v>
       </c>
-      <c r="E17" s="4">
+      <c r="E17" s="3">
         <v>1E-3</v>
       </c>
-      <c r="F17" s="4">
+      <c r="F17" s="3">
         <v>2E-3</v>
       </c>
-      <c r="G17" s="4">
+      <c r="G17" s="3">
         <v>3.0000000000000001E-3</v>
       </c>
       <c r="H17" t="s">
@@ -2311,7 +2311,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2B79E74F-84B4-4DAF-A8CA-9F8B24A5CC9D}">
   <dimension ref="A1:R26"/>
   <sheetViews>
-    <sheetView topLeftCell="A5" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="Q21" sqref="Q21"/>
     </sheetView>
   </sheetViews>
@@ -2381,55 +2381,55 @@
       <c r="A2" t="s">
         <v>19</v>
       </c>
-      <c r="B2" s="4">
+      <c r="B2" s="3">
         <v>0.19500000000000001</v>
       </c>
       <c r="C2" t="s">
         <v>28</v>
       </c>
-      <c r="D2" s="4">
+      <c r="D2" s="3">
         <v>0.24</v>
       </c>
-      <c r="E2" s="4">
+      <c r="E2" s="3">
         <v>0.26500000000000001</v>
       </c>
-      <c r="F2" s="4">
+      <c r="F2" s="3">
         <v>0.29899999999999999</v>
       </c>
-      <c r="G2" s="4">
+      <c r="G2" s="3">
         <v>0.246</v>
       </c>
-      <c r="H2" s="4">
+      <c r="H2" s="3">
         <v>0.29599999999999999</v>
       </c>
-      <c r="I2" s="4">
+      <c r="I2" s="3">
         <v>0.29199999999999998</v>
       </c>
-      <c r="J2" s="4">
+      <c r="J2" s="3">
         <v>0.29799999999999999</v>
       </c>
-      <c r="K2" s="4">
+      <c r="K2" s="3">
         <v>0.29899999999999999</v>
       </c>
-      <c r="L2" s="4">
+      <c r="L2" s="3">
         <v>0.311</v>
       </c>
-      <c r="M2" s="4">
+      <c r="M2" s="3">
         <v>0.29699999999999999</v>
       </c>
-      <c r="N2" s="4">
+      <c r="N2" s="3">
         <v>0.31</v>
       </c>
-      <c r="O2" s="4">
+      <c r="O2" s="3">
         <v>0.31</v>
       </c>
-      <c r="P2" s="4">
+      <c r="P2" s="3">
         <v>0.34</v>
       </c>
-      <c r="Q2" s="4">
+      <c r="Q2" s="3">
         <v>0.33</v>
       </c>
-      <c r="R2" s="4">
+      <c r="R2" s="3">
         <v>0.31</v>
       </c>
     </row>
@@ -2437,40 +2437,40 @@
       <c r="A3" t="s">
         <v>20</v>
       </c>
-      <c r="B3" s="4">
+      <c r="B3" s="3">
         <v>0.14799999999999999</v>
       </c>
       <c r="C3" t="s">
         <v>20</v>
       </c>
-      <c r="D3" s="4">
+      <c r="D3" s="3">
         <v>0.111</v>
       </c>
-      <c r="E3" s="4">
+      <c r="E3" s="3">
         <v>0.109</v>
       </c>
-      <c r="F3" s="4">
+      <c r="F3" s="3">
         <v>0.104</v>
       </c>
-      <c r="G3" s="4">
+      <c r="G3" s="3">
         <v>8.8999999999999996E-2</v>
       </c>
-      <c r="H3" s="4">
+      <c r="H3" s="3">
         <v>0.10100000000000001</v>
       </c>
-      <c r="I3" s="4">
+      <c r="I3" s="3">
         <v>0.112</v>
       </c>
-      <c r="J3" s="4">
+      <c r="J3" s="3">
         <v>0.109</v>
       </c>
-      <c r="K3" s="4">
+      <c r="K3" s="3">
         <v>0.121</v>
       </c>
-      <c r="L3" s="4">
+      <c r="L3" s="3">
         <v>0.105</v>
       </c>
-      <c r="M3" s="4">
+      <c r="M3" s="3">
         <v>9.7000000000000003E-2</v>
       </c>
       <c r="N3" t="s">
@@ -2493,40 +2493,40 @@
       <c r="A4" t="s">
         <v>21</v>
       </c>
-      <c r="B4" s="4">
+      <c r="B4" s="3">
         <v>0.26</v>
       </c>
       <c r="C4" t="s">
         <v>29</v>
       </c>
-      <c r="D4" s="4">
+      <c r="D4" s="3">
         <v>0.21299999999999999</v>
       </c>
-      <c r="E4" s="4">
+      <c r="E4" s="3">
         <v>0.21199999999999999</v>
       </c>
-      <c r="F4" s="4">
+      <c r="F4" s="3">
         <v>0.223</v>
       </c>
-      <c r="G4" s="4">
+      <c r="G4" s="3">
         <v>0.19500000000000001</v>
       </c>
-      <c r="H4" s="4">
+      <c r="H4" s="3">
         <v>0.19400000000000001</v>
       </c>
-      <c r="I4" s="4">
+      <c r="I4" s="3">
         <v>0.20200000000000001</v>
       </c>
-      <c r="J4" s="4">
+      <c r="J4" s="3">
         <v>0.19800000000000001</v>
       </c>
-      <c r="K4" s="4">
+      <c r="K4" s="3">
         <v>0.19</v>
       </c>
-      <c r="L4" s="4">
+      <c r="L4" s="3">
         <v>0.2</v>
       </c>
-      <c r="M4" s="4">
+      <c r="M4" s="3">
         <v>0.19500000000000001</v>
       </c>
       <c r="N4" t="s">
@@ -2549,55 +2549,55 @@
       <c r="A5" t="s">
         <v>22</v>
       </c>
-      <c r="B5" s="4">
+      <c r="B5" s="3">
         <v>0.23200000000000001</v>
       </c>
-      <c r="C5" s="3" t="s">
+      <c r="C5" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="D5" s="5">
+      <c r="D5" s="6">
         <v>0.30199999999999999</v>
       </c>
-      <c r="E5" s="5">
+      <c r="E5" s="6">
         <v>0.30099999999999999</v>
       </c>
-      <c r="F5" s="5">
+      <c r="F5" s="6">
         <v>0.28899999999999998</v>
       </c>
-      <c r="G5" s="5">
+      <c r="G5" s="6">
         <v>0.34599999999999997</v>
       </c>
-      <c r="H5" s="5">
+      <c r="H5" s="6">
         <v>0.315</v>
       </c>
-      <c r="I5" s="5">
+      <c r="I5" s="6">
         <v>0.29299999999999998</v>
       </c>
-      <c r="J5" s="5">
+      <c r="J5" s="6">
         <v>0.33900000000000002</v>
       </c>
-      <c r="K5" s="5">
+      <c r="K5" s="6">
         <v>0.32600000000000001</v>
       </c>
-      <c r="L5" s="5">
+      <c r="L5" s="6">
         <v>0.316</v>
       </c>
-      <c r="M5" s="5">
+      <c r="M5" s="6">
         <v>0.35499999999999998</v>
       </c>
-      <c r="N5" s="5">
+      <c r="N5" s="6">
         <v>0.35</v>
       </c>
-      <c r="O5" s="5">
+      <c r="O5" s="6">
         <v>0.36</v>
       </c>
-      <c r="P5" s="5">
+      <c r="P5" s="6">
         <v>0.3</v>
       </c>
-      <c r="Q5" s="5">
+      <c r="Q5" s="6">
         <v>0.35</v>
       </c>
-      <c r="R5" s="5">
+      <c r="R5" s="6">
         <v>0.34</v>
       </c>
     </row>
@@ -2605,79 +2605,79 @@
       <c r="A6" t="s">
         <v>23</v>
       </c>
-      <c r="B6" s="4">
+      <c r="B6" s="3">
         <v>2.5999999999999999E-2</v>
       </c>
-      <c r="C6" s="3"/>
-      <c r="D6" s="5"/>
-      <c r="E6" s="5"/>
-      <c r="F6" s="5"/>
-      <c r="G6" s="5"/>
-      <c r="H6" s="5"/>
-      <c r="I6" s="5"/>
-      <c r="J6" s="5"/>
-      <c r="K6" s="5"/>
-      <c r="L6" s="5"/>
-      <c r="M6" s="5"/>
-      <c r="N6" s="5"/>
-      <c r="O6" s="5"/>
-      <c r="P6" s="5"/>
-      <c r="Q6" s="5"/>
-      <c r="R6" s="5"/>
+      <c r="C6" s="5"/>
+      <c r="D6" s="6"/>
+      <c r="E6" s="6"/>
+      <c r="F6" s="6"/>
+      <c r="G6" s="6"/>
+      <c r="H6" s="6"/>
+      <c r="I6" s="6"/>
+      <c r="J6" s="6"/>
+      <c r="K6" s="6"/>
+      <c r="L6" s="6"/>
+      <c r="M6" s="6"/>
+      <c r="N6" s="6"/>
+      <c r="O6" s="6"/>
+      <c r="P6" s="6"/>
+      <c r="Q6" s="6"/>
+      <c r="R6" s="6"/>
     </row>
     <row r="7" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>24</v>
       </c>
-      <c r="B7" s="4">
+      <c r="B7" s="3">
         <v>9.6000000000000002E-2</v>
       </c>
-      <c r="C7" s="3" t="s">
+      <c r="C7" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="D7" s="5">
+      <c r="D7" s="6">
         <v>0.13400000000000001</v>
       </c>
-      <c r="E7" s="5">
+      <c r="E7" s="6">
         <v>0.113</v>
       </c>
-      <c r="F7" s="5">
+      <c r="F7" s="6">
         <v>8.5000000000000006E-2</v>
       </c>
-      <c r="G7" s="5">
+      <c r="G7" s="6">
         <v>0.124</v>
       </c>
-      <c r="H7" s="5">
+      <c r="H7" s="6">
         <v>9.5000000000000001E-2</v>
       </c>
-      <c r="I7" s="5">
+      <c r="I7" s="6">
         <v>0.1</v>
       </c>
-      <c r="J7" s="5">
+      <c r="J7" s="6">
         <v>5.6000000000000001E-2</v>
       </c>
-      <c r="K7" s="5">
+      <c r="K7" s="6">
         <v>6.4000000000000001E-2</v>
       </c>
-      <c r="L7" s="5">
+      <c r="L7" s="6">
         <v>6.8000000000000005E-2</v>
       </c>
-      <c r="M7" s="5">
+      <c r="M7" s="6">
         <v>5.5E-2</v>
       </c>
-      <c r="N7" s="5">
+      <c r="N7" s="6">
         <v>0.04</v>
       </c>
-      <c r="O7" s="5">
+      <c r="O7" s="6">
         <v>0.04</v>
       </c>
-      <c r="P7" s="5">
+      <c r="P7" s="6">
         <v>0.04</v>
       </c>
-      <c r="Q7" s="5">
+      <c r="Q7" s="6">
         <v>0.03</v>
       </c>
-      <c r="R7" s="5">
+      <c r="R7" s="6">
         <v>0.03</v>
       </c>
     </row>
@@ -2685,25 +2685,25 @@
       <c r="A8" t="s">
         <v>25</v>
       </c>
-      <c r="B8" s="4">
+      <c r="B8" s="3">
         <v>4.3999999999999997E-2</v>
       </c>
-      <c r="C8" s="3"/>
-      <c r="D8" s="5"/>
-      <c r="E8" s="5"/>
-      <c r="F8" s="5"/>
-      <c r="G8" s="5"/>
-      <c r="H8" s="5"/>
-      <c r="I8" s="5"/>
-      <c r="J8" s="5"/>
-      <c r="K8" s="5"/>
-      <c r="L8" s="5"/>
-      <c r="M8" s="5"/>
-      <c r="N8" s="5"/>
-      <c r="O8" s="5"/>
-      <c r="P8" s="5"/>
-      <c r="Q8" s="5"/>
-      <c r="R8" s="5"/>
+      <c r="C8" s="5"/>
+      <c r="D8" s="6"/>
+      <c r="E8" s="6"/>
+      <c r="F8" s="6"/>
+      <c r="G8" s="6"/>
+      <c r="H8" s="6"/>
+      <c r="I8" s="6"/>
+      <c r="J8" s="6"/>
+      <c r="K8" s="6"/>
+      <c r="L8" s="6"/>
+      <c r="M8" s="6"/>
+      <c r="N8" s="6"/>
+      <c r="O8" s="6"/>
+      <c r="P8" s="6"/>
+      <c r="Q8" s="6"/>
+      <c r="R8" s="6"/>
     </row>
     <row r="10" spans="1:18" ht="16.5" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
@@ -2765,55 +2765,55 @@
       <c r="A11" t="s">
         <v>19</v>
       </c>
-      <c r="B11" s="4">
+      <c r="B11" s="3">
         <v>3.4000000000000002E-2</v>
       </c>
       <c r="C11" t="s">
         <v>28</v>
       </c>
-      <c r="D11" s="4">
-        <v>0</v>
-      </c>
-      <c r="E11" s="4">
-        <v>0</v>
-      </c>
-      <c r="F11" s="4">
+      <c r="D11" s="3">
+        <v>0</v>
+      </c>
+      <c r="E11" s="3">
+        <v>0</v>
+      </c>
+      <c r="F11" s="3">
         <v>1.2E-2</v>
       </c>
-      <c r="G11" s="4">
+      <c r="G11" s="3">
         <v>1E-3</v>
       </c>
-      <c r="H11" s="4">
+      <c r="H11" s="3">
         <v>1E-3</v>
       </c>
-      <c r="I11" s="4">
+      <c r="I11" s="3">
         <v>3.0000000000000001E-3</v>
       </c>
-      <c r="J11" s="4">
+      <c r="J11" s="3">
         <v>2E-3</v>
       </c>
-      <c r="K11" s="4">
+      <c r="K11" s="3">
         <v>1.0999999999999999E-2</v>
       </c>
-      <c r="L11" s="4">
+      <c r="L11" s="3">
         <v>2E-3</v>
       </c>
-      <c r="M11" s="4">
+      <c r="M11" s="3">
         <v>3.1E-2</v>
       </c>
       <c r="N11" t="s">
         <v>0</v>
       </c>
-      <c r="O11" s="4">
+      <c r="O11" s="3">
         <v>0.02</v>
       </c>
-      <c r="P11" s="4">
+      <c r="P11" s="3">
         <v>0.02</v>
       </c>
-      <c r="Q11" s="4">
+      <c r="Q11" s="3">
         <v>8.9999999999999993E-3</v>
       </c>
-      <c r="R11" s="4">
+      <c r="R11" s="3">
         <v>2.3E-2</v>
       </c>
     </row>
@@ -2821,40 +2821,40 @@
       <c r="A12" t="s">
         <v>20</v>
       </c>
-      <c r="B12" s="4">
+      <c r="B12" s="3">
         <v>0.17</v>
       </c>
       <c r="C12" t="s">
         <v>20</v>
       </c>
-      <c r="D12" s="4">
+      <c r="D12" s="3">
         <v>2.9000000000000001E-2</v>
       </c>
-      <c r="E12" s="4">
+      <c r="E12" s="3">
         <v>3.3000000000000002E-2</v>
       </c>
-      <c r="F12" s="4">
+      <c r="F12" s="3">
         <v>6.0999999999999999E-2</v>
       </c>
-      <c r="G12" s="4">
+      <c r="G12" s="3">
         <v>2.7E-2</v>
       </c>
-      <c r="H12" s="4">
+      <c r="H12" s="3">
         <v>0.05</v>
       </c>
-      <c r="I12" s="4">
+      <c r="I12" s="3">
         <v>0.04</v>
       </c>
-      <c r="J12" s="4">
+      <c r="J12" s="3">
         <v>2.1000000000000001E-2</v>
       </c>
-      <c r="K12" s="4">
+      <c r="K12" s="3">
         <v>5.5E-2</v>
       </c>
-      <c r="L12" s="4">
+      <c r="L12" s="3">
         <v>8.3000000000000004E-2</v>
       </c>
-      <c r="M12" s="4">
+      <c r="M12" s="3">
         <v>0.124</v>
       </c>
       <c r="N12" t="s">
@@ -2877,40 +2877,40 @@
       <c r="A13" t="s">
         <v>21</v>
       </c>
-      <c r="B13" s="4">
+      <c r="B13" s="3">
         <v>0.254</v>
       </c>
       <c r="C13" t="s">
         <v>29</v>
       </c>
-      <c r="D13" s="4">
+      <c r="D13" s="3">
         <v>0.34</v>
       </c>
-      <c r="E13" s="4">
+      <c r="E13" s="3">
         <v>0.33100000000000002</v>
       </c>
-      <c r="F13" s="4">
+      <c r="F13" s="3">
         <v>0.32800000000000001</v>
       </c>
-      <c r="G13" s="4">
+      <c r="G13" s="3">
         <v>0.35</v>
       </c>
-      <c r="H13" s="4">
+      <c r="H13" s="3">
         <v>0.34699999999999998</v>
       </c>
-      <c r="I13" s="4">
+      <c r="I13" s="3">
         <v>0.38100000000000001</v>
       </c>
-      <c r="J13" s="4">
+      <c r="J13" s="3">
         <v>0.28199999999999997</v>
       </c>
-      <c r="K13" s="4">
+      <c r="K13" s="3">
         <v>0.33300000000000002</v>
       </c>
-      <c r="L13" s="4">
+      <c r="L13" s="3">
         <v>0.30499999999999999</v>
       </c>
-      <c r="M13" s="4">
+      <c r="M13" s="3">
         <v>0.30199999999999999</v>
       </c>
       <c r="N13" t="s">
@@ -2933,55 +2933,55 @@
       <c r="A14" t="s">
         <v>22</v>
       </c>
-      <c r="B14" s="4">
+      <c r="B14" s="3">
         <v>0.314</v>
       </c>
-      <c r="C14" s="3" t="s">
+      <c r="C14" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="D14" s="5">
+      <c r="D14" s="6">
         <v>0.55300000000000005</v>
       </c>
-      <c r="E14" s="5">
+      <c r="E14" s="6">
         <v>0.435</v>
       </c>
-      <c r="F14" s="5">
+      <c r="F14" s="6">
         <v>0.45600000000000002</v>
       </c>
-      <c r="G14" s="5">
+      <c r="G14" s="6">
         <v>0.501</v>
       </c>
-      <c r="H14" s="5">
+      <c r="H14" s="6">
         <v>0.47399999999999998</v>
       </c>
-      <c r="I14" s="5">
+      <c r="I14" s="6">
         <v>0.46700000000000003</v>
       </c>
-      <c r="J14" s="5">
+      <c r="J14" s="6">
         <v>0.58299999999999996</v>
       </c>
-      <c r="K14" s="5">
+      <c r="K14" s="6">
         <v>0.52100000000000002</v>
       </c>
-      <c r="L14" s="5">
+      <c r="L14" s="6">
         <v>0.53700000000000003</v>
       </c>
-      <c r="M14" s="5">
+      <c r="M14" s="6">
         <v>0.434</v>
       </c>
-      <c r="N14" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="O14" s="5">
+      <c r="N14" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="O14" s="6">
         <v>0.44</v>
       </c>
-      <c r="P14" s="5">
+      <c r="P14" s="6">
         <v>0.53</v>
       </c>
-      <c r="Q14" s="5">
+      <c r="Q14" s="6">
         <v>0.49</v>
       </c>
-      <c r="R14" s="5">
+      <c r="R14" s="6">
         <v>0.47</v>
       </c>
     </row>
@@ -2989,79 +2989,79 @@
       <c r="A15" t="s">
         <v>23</v>
       </c>
-      <c r="B15" s="4">
+      <c r="B15" s="3">
         <v>0.19600000000000001</v>
       </c>
-      <c r="C15" s="3"/>
-      <c r="D15" s="5"/>
-      <c r="E15" s="5"/>
-      <c r="F15" s="5"/>
-      <c r="G15" s="5"/>
-      <c r="H15" s="5"/>
-      <c r="I15" s="5"/>
-      <c r="J15" s="5"/>
-      <c r="K15" s="5"/>
-      <c r="L15" s="5"/>
-      <c r="M15" s="5"/>
-      <c r="N15" s="3"/>
-      <c r="O15" s="5"/>
-      <c r="P15" s="5"/>
-      <c r="Q15" s="5"/>
-      <c r="R15" s="5"/>
+      <c r="C15" s="5"/>
+      <c r="D15" s="6"/>
+      <c r="E15" s="6"/>
+      <c r="F15" s="6"/>
+      <c r="G15" s="6"/>
+      <c r="H15" s="6"/>
+      <c r="I15" s="6"/>
+      <c r="J15" s="6"/>
+      <c r="K15" s="6"/>
+      <c r="L15" s="6"/>
+      <c r="M15" s="6"/>
+      <c r="N15" s="5"/>
+      <c r="O15" s="6"/>
+      <c r="P15" s="6"/>
+      <c r="Q15" s="6"/>
+      <c r="R15" s="6"/>
     </row>
     <row r="16" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>24</v>
       </c>
-      <c r="B16" s="4">
+      <c r="B16" s="3">
         <v>3.1E-2</v>
       </c>
-      <c r="C16" s="3" t="s">
+      <c r="C16" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="D16" s="5">
+      <c r="D16" s="6">
         <v>7.8E-2</v>
       </c>
-      <c r="E16" s="5">
+      <c r="E16" s="6">
         <v>0.20100000000000001</v>
       </c>
-      <c r="F16" s="5">
+      <c r="F16" s="6">
         <v>0.14399999999999999</v>
       </c>
-      <c r="G16" s="5">
+      <c r="G16" s="6">
         <v>0.121</v>
       </c>
-      <c r="H16" s="5">
+      <c r="H16" s="6">
         <v>0.128</v>
       </c>
-      <c r="I16" s="5">
+      <c r="I16" s="6">
         <v>0.108</v>
       </c>
-      <c r="J16" s="5">
+      <c r="J16" s="6">
         <v>0.112</v>
       </c>
-      <c r="K16" s="5">
+      <c r="K16" s="6">
         <v>0.08</v>
       </c>
-      <c r="L16" s="5">
+      <c r="L16" s="6">
         <v>7.1999999999999995E-2</v>
       </c>
-      <c r="M16" s="5">
+      <c r="M16" s="6">
         <v>0.109</v>
       </c>
-      <c r="N16" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="O16" s="5">
+      <c r="N16" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="O16" s="6">
         <v>0.09</v>
       </c>
-      <c r="P16" s="5">
+      <c r="P16" s="6">
         <v>0.04</v>
       </c>
-      <c r="Q16" s="5">
+      <c r="Q16" s="6">
         <v>0.06</v>
       </c>
-      <c r="R16" s="5">
+      <c r="R16" s="6">
         <v>0.04</v>
       </c>
     </row>
@@ -3069,25 +3069,25 @@
       <c r="A17" t="s">
         <v>25</v>
       </c>
-      <c r="B17" s="4">
+      <c r="B17" s="3">
         <v>1E-3</v>
       </c>
-      <c r="C17" s="3"/>
-      <c r="D17" s="5"/>
-      <c r="E17" s="5"/>
-      <c r="F17" s="5"/>
-      <c r="G17" s="5"/>
-      <c r="H17" s="5"/>
-      <c r="I17" s="5"/>
-      <c r="J17" s="5"/>
-      <c r="K17" s="5"/>
-      <c r="L17" s="5"/>
-      <c r="M17" s="5"/>
-      <c r="N17" s="3"/>
-      <c r="O17" s="5"/>
-      <c r="P17" s="5"/>
-      <c r="Q17" s="5"/>
-      <c r="R17" s="5"/>
+      <c r="C17" s="5"/>
+      <c r="D17" s="6"/>
+      <c r="E17" s="6"/>
+      <c r="F17" s="6"/>
+      <c r="G17" s="6"/>
+      <c r="H17" s="6"/>
+      <c r="I17" s="6"/>
+      <c r="J17" s="6"/>
+      <c r="K17" s="6"/>
+      <c r="L17" s="6"/>
+      <c r="M17" s="6"/>
+      <c r="N17" s="5"/>
+      <c r="O17" s="6"/>
+      <c r="P17" s="6"/>
+      <c r="Q17" s="6"/>
+      <c r="R17" s="6"/>
     </row>
     <row r="19" spans="1:18" ht="16.5" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
@@ -3149,55 +3149,55 @@
       <c r="A20" t="s">
         <v>19</v>
       </c>
-      <c r="B20" s="4">
+      <c r="B20" s="3">
         <v>0.16300000000000001</v>
       </c>
       <c r="C20" t="s">
         <v>28</v>
       </c>
-      <c r="D20" s="4">
+      <c r="D20" s="3">
         <v>0.16200000000000001</v>
       </c>
-      <c r="E20" s="4">
+      <c r="E20" s="3">
         <v>0.215</v>
       </c>
-      <c r="F20" s="4">
+      <c r="F20" s="3">
         <v>0.21</v>
       </c>
-      <c r="G20" s="4">
+      <c r="G20" s="3">
         <v>0.20100000000000001</v>
       </c>
-      <c r="H20" s="4">
+      <c r="H20" s="3">
         <v>0.223</v>
       </c>
-      <c r="I20" s="4">
+      <c r="I20" s="3">
         <v>0.21299999999999999</v>
       </c>
-      <c r="J20" s="4">
+      <c r="J20" s="3">
         <v>0.23599999999999999</v>
       </c>
-      <c r="K20" s="4">
+      <c r="K20" s="3">
         <v>0.21199999999999999</v>
       </c>
-      <c r="L20" s="4">
+      <c r="L20" s="3">
         <v>0.26800000000000002</v>
       </c>
-      <c r="M20" s="4">
+      <c r="M20" s="3">
         <v>3.1E-2</v>
       </c>
       <c r="N20" t="s">
         <v>0</v>
       </c>
-      <c r="O20" s="4">
+      <c r="O20" s="3">
         <v>0.28000000000000003</v>
       </c>
-      <c r="P20" s="4">
+      <c r="P20" s="3">
         <v>0.28000000000000003</v>
       </c>
-      <c r="Q20" s="4">
+      <c r="Q20" s="3">
         <v>0.25</v>
       </c>
-      <c r="R20" s="4">
+      <c r="R20" s="3">
         <v>0.26</v>
       </c>
     </row>
@@ -3205,40 +3205,40 @@
       <c r="A21" t="s">
         <v>20</v>
       </c>
-      <c r="B21" s="4">
+      <c r="B21" s="3">
         <v>0.129</v>
       </c>
       <c r="C21" t="s">
         <v>20</v>
       </c>
-      <c r="D21" s="4">
+      <c r="D21" s="3">
         <v>8.5000000000000006E-2</v>
       </c>
-      <c r="E21" s="4">
+      <c r="E21" s="3">
         <v>9.5000000000000001E-2</v>
       </c>
-      <c r="F21" s="4">
+      <c r="F21" s="3">
         <v>9.1999999999999998E-2</v>
       </c>
-      <c r="G21" s="4">
+      <c r="G21" s="3">
         <v>7.6999999999999999E-2</v>
       </c>
-      <c r="H21" s="4">
+      <c r="H21" s="3">
         <v>8.7999999999999995E-2</v>
       </c>
-      <c r="I21" s="4">
+      <c r="I21" s="3">
         <v>9.1999999999999998E-2</v>
       </c>
-      <c r="J21" s="4">
+      <c r="J21" s="3">
         <v>0.09</v>
       </c>
-      <c r="K21" s="4">
+      <c r="K21" s="3">
         <v>0.10100000000000001</v>
       </c>
-      <c r="L21" s="4">
+      <c r="L21" s="3">
         <v>0.10199999999999999</v>
       </c>
-      <c r="M21" s="4">
+      <c r="M21" s="3">
         <v>0.124</v>
       </c>
       <c r="N21" t="s">
@@ -3261,40 +3261,40 @@
       <c r="A22" t="s">
         <v>21</v>
       </c>
-      <c r="B22" s="4">
+      <c r="B22" s="3">
         <v>0.245</v>
       </c>
       <c r="C22" t="s">
         <v>29</v>
       </c>
-      <c r="D22" s="4">
+      <c r="D22" s="3">
         <v>0.254</v>
       </c>
-      <c r="E22" s="4">
+      <c r="E22" s="3">
         <v>0.23499999999999999</v>
       </c>
-      <c r="F22" s="4">
+      <c r="F22" s="3">
         <v>0.25600000000000001</v>
       </c>
-      <c r="G22" s="4">
+      <c r="G22" s="3">
         <v>0.224</v>
       </c>
-      <c r="H22" s="4">
+      <c r="H22" s="3">
         <v>0.23200000000000001</v>
       </c>
-      <c r="I22" s="4">
+      <c r="I22" s="3">
         <v>0.251</v>
       </c>
-      <c r="J22" s="4">
+      <c r="J22" s="3">
         <v>0.216</v>
       </c>
-      <c r="K22" s="4">
+      <c r="K22" s="3">
         <v>0.23400000000000001</v>
       </c>
-      <c r="L22" s="4">
+      <c r="L22" s="3">
         <v>0.215</v>
       </c>
-      <c r="M22" s="4">
+      <c r="M22" s="3">
         <v>0.30199999999999999</v>
       </c>
       <c r="N22" t="s">
@@ -3317,55 +3317,55 @@
       <c r="A23" t="s">
         <v>22</v>
       </c>
-      <c r="B23" s="4">
+      <c r="B23" s="3">
         <v>0.23599999999999999</v>
       </c>
-      <c r="C23" s="3" t="s">
+      <c r="C23" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="D23" s="4">
+      <c r="D23" s="3">
         <v>0.38400000000000001</v>
       </c>
-      <c r="E23" s="4">
+      <c r="E23" s="3">
         <v>0.32600000000000001</v>
       </c>
-      <c r="F23" s="4">
+      <c r="F23" s="3">
         <v>0.34</v>
       </c>
-      <c r="G23" s="4">
+      <c r="G23" s="3">
         <v>0.374</v>
       </c>
-      <c r="H23" s="4">
+      <c r="H23" s="3">
         <v>0.35499999999999998</v>
       </c>
-      <c r="I23" s="4">
+      <c r="I23" s="3">
         <v>0.34100000000000003</v>
       </c>
-      <c r="J23" s="4">
+      <c r="J23" s="3">
         <v>0.39</v>
       </c>
-      <c r="K23" s="4">
+      <c r="K23" s="3">
         <v>0.38500000000000001</v>
       </c>
-      <c r="L23" s="4">
+      <c r="L23" s="3">
         <v>0.34699999999999998</v>
       </c>
-      <c r="M23" s="4">
+      <c r="M23" s="3">
         <v>0.434</v>
       </c>
       <c r="N23" t="s">
         <v>0</v>
       </c>
-      <c r="O23" s="4">
+      <c r="O23" s="3">
         <v>0.35</v>
       </c>
-      <c r="P23" s="4">
+      <c r="P23" s="3">
         <v>0.35</v>
       </c>
-      <c r="Q23" s="4">
+      <c r="Q23" s="3">
         <v>0.38</v>
       </c>
-      <c r="R23" s="4">
+      <c r="R23" s="3">
         <v>0.37</v>
       </c>
     </row>
@@ -3373,53 +3373,53 @@
       <c r="A24" t="s">
         <v>23</v>
       </c>
-      <c r="B24" s="4">
+      <c r="B24" s="3">
         <v>7.2999999999999995E-2</v>
       </c>
-      <c r="C24" s="3"/>
-      <c r="D24" s="4">
+      <c r="C24" s="5"/>
+      <c r="D24" s="3">
         <v>0.11600000000000001</v>
       </c>
-      <c r="E24" s="4">
+      <c r="E24" s="3">
         <v>0.129</v>
       </c>
-      <c r="F24" s="4">
+      <c r="F24" s="3">
         <v>0.10199999999999999</v>
       </c>
-      <c r="G24" s="4">
+      <c r="G24" s="3">
         <v>0.123</v>
       </c>
-      <c r="H24" s="4">
+      <c r="H24" s="3">
         <v>0.10299999999999999</v>
       </c>
-      <c r="I24" s="4">
+      <c r="I24" s="3">
         <v>0.10299999999999999</v>
       </c>
-      <c r="J24" s="4">
+      <c r="J24" s="3">
         <v>6.8000000000000005E-2</v>
       </c>
-      <c r="K24" s="4">
+      <c r="K24" s="3">
         <v>6.8000000000000005E-2</v>
       </c>
-      <c r="L24" s="4">
+      <c r="L24" s="3">
         <v>6.8000000000000005E-2</v>
       </c>
-      <c r="M24" s="4">
+      <c r="M24" s="3">
         <v>0.109</v>
       </c>
       <c r="N24" t="s">
         <v>0</v>
       </c>
-      <c r="O24" s="4">
+      <c r="O24" s="3">
         <v>0.04</v>
       </c>
-      <c r="P24" s="4">
+      <c r="P24" s="3">
         <v>0.04</v>
       </c>
-      <c r="Q24" s="4">
+      <c r="Q24" s="3">
         <v>0.04</v>
       </c>
-      <c r="R24" s="4">
+      <c r="R24" s="3">
         <v>0.03</v>
       </c>
     </row>
@@ -3427,55 +3427,55 @@
       <c r="A25" t="s">
         <v>24</v>
       </c>
-      <c r="B25" s="4">
+      <c r="B25" s="3">
         <v>0.112</v>
       </c>
-      <c r="C25" s="3" t="s">
+      <c r="C25" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="D25" s="5">
+      <c r="D25" s="6">
         <v>0.11600000000000001</v>
       </c>
-      <c r="E25" s="5">
+      <c r="E25" s="6">
         <v>0.129</v>
       </c>
-      <c r="F25" s="5">
+      <c r="F25" s="6">
         <v>0.10199999999999999</v>
       </c>
-      <c r="G25" s="5">
+      <c r="G25" s="6">
         <v>0.123</v>
       </c>
-      <c r="H25" s="5">
+      <c r="H25" s="6">
         <v>0.10299999999999999</v>
       </c>
-      <c r="I25" s="5">
+      <c r="I25" s="6">
         <v>0.10299999999999999</v>
       </c>
-      <c r="J25" s="5">
+      <c r="J25" s="6">
         <v>6.8000000000000005E-2</v>
       </c>
-      <c r="K25" s="5">
+      <c r="K25" s="6">
         <v>6.8000000000000005E-2</v>
       </c>
-      <c r="L25" s="5">
+      <c r="L25" s="6">
         <v>6.8000000000000005E-2</v>
       </c>
-      <c r="M25" s="5">
+      <c r="M25" s="6">
         <v>0.109</v>
       </c>
-      <c r="N25" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="O25" s="5">
+      <c r="N25" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="O25" s="6">
         <v>0.04</v>
       </c>
-      <c r="P25" s="5">
+      <c r="P25" s="6">
         <v>0.04</v>
       </c>
-      <c r="Q25" s="5">
+      <c r="Q25" s="6">
         <v>0.04</v>
       </c>
-      <c r="R25" s="5">
+      <c r="R25" s="6">
         <v>0.03</v>
       </c>
     </row>
@@ -3483,37 +3483,84 @@
       <c r="A26" t="s">
         <v>25</v>
       </c>
-      <c r="B26" s="4">
+      <c r="B26" s="3">
         <v>4.2000000000000003E-2</v>
       </c>
-      <c r="C26" s="3"/>
-      <c r="D26" s="5"/>
-      <c r="E26" s="5"/>
-      <c r="F26" s="5"/>
-      <c r="G26" s="5"/>
-      <c r="H26" s="5"/>
-      <c r="I26" s="5"/>
-      <c r="J26" s="5"/>
-      <c r="K26" s="5"/>
-      <c r="L26" s="5"/>
-      <c r="M26" s="5"/>
-      <c r="N26" s="3"/>
-      <c r="O26" s="5"/>
-      <c r="P26" s="5"/>
-      <c r="Q26" s="5"/>
-      <c r="R26" s="5"/>
+      <c r="C26" s="5"/>
+      <c r="D26" s="6"/>
+      <c r="E26" s="6"/>
+      <c r="F26" s="6"/>
+      <c r="G26" s="6"/>
+      <c r="H26" s="6"/>
+      <c r="I26" s="6"/>
+      <c r="J26" s="6"/>
+      <c r="K26" s="6"/>
+      <c r="L26" s="6"/>
+      <c r="M26" s="6"/>
+      <c r="N26" s="5"/>
+      <c r="O26" s="6"/>
+      <c r="P26" s="6"/>
+      <c r="Q26" s="6"/>
+      <c r="R26" s="6"/>
     </row>
   </sheetData>
   <mergeCells count="81">
-    <mergeCell ref="P25:P26"/>
-    <mergeCell ref="Q25:Q26"/>
-    <mergeCell ref="R25:R26"/>
-    <mergeCell ref="J25:J26"/>
-    <mergeCell ref="K25:K26"/>
-    <mergeCell ref="L25:L26"/>
-    <mergeCell ref="M25:M26"/>
-    <mergeCell ref="N25:N26"/>
-    <mergeCell ref="O25:O26"/>
+    <mergeCell ref="C5:C6"/>
+    <mergeCell ref="C7:C8"/>
+    <mergeCell ref="D5:D6"/>
+    <mergeCell ref="D7:D8"/>
+    <mergeCell ref="E5:E6"/>
+    <mergeCell ref="E7:E8"/>
+    <mergeCell ref="F5:F6"/>
+    <mergeCell ref="F7:F8"/>
+    <mergeCell ref="G5:G6"/>
+    <mergeCell ref="G7:G8"/>
+    <mergeCell ref="H5:H6"/>
+    <mergeCell ref="H7:H8"/>
+    <mergeCell ref="I5:I6"/>
+    <mergeCell ref="I7:I8"/>
+    <mergeCell ref="J5:J6"/>
+    <mergeCell ref="J7:J8"/>
+    <mergeCell ref="K5:K6"/>
+    <mergeCell ref="K7:K8"/>
+    <mergeCell ref="L5:L6"/>
+    <mergeCell ref="L7:L8"/>
+    <mergeCell ref="M5:M6"/>
+    <mergeCell ref="M7:M8"/>
+    <mergeCell ref="N5:N6"/>
+    <mergeCell ref="N7:N8"/>
+    <mergeCell ref="R5:R6"/>
+    <mergeCell ref="R7:R8"/>
+    <mergeCell ref="C14:C15"/>
+    <mergeCell ref="C16:C17"/>
+    <mergeCell ref="D14:D15"/>
+    <mergeCell ref="E14:E15"/>
+    <mergeCell ref="F14:F15"/>
+    <mergeCell ref="G14:G15"/>
+    <mergeCell ref="H14:H15"/>
+    <mergeCell ref="I14:I15"/>
+    <mergeCell ref="O5:O6"/>
+    <mergeCell ref="O7:O8"/>
+    <mergeCell ref="P5:P6"/>
+    <mergeCell ref="P7:P8"/>
+    <mergeCell ref="Q5:Q6"/>
+    <mergeCell ref="Q7:Q8"/>
+    <mergeCell ref="P14:P15"/>
+    <mergeCell ref="Q14:Q15"/>
+    <mergeCell ref="R14:R15"/>
+    <mergeCell ref="D16:D17"/>
+    <mergeCell ref="E16:E17"/>
+    <mergeCell ref="F16:F17"/>
+    <mergeCell ref="G16:G17"/>
+    <mergeCell ref="H16:H17"/>
+    <mergeCell ref="I16:I17"/>
+    <mergeCell ref="J16:J17"/>
+    <mergeCell ref="J14:J15"/>
+    <mergeCell ref="K14:K15"/>
+    <mergeCell ref="L14:L15"/>
+    <mergeCell ref="M14:M15"/>
+    <mergeCell ref="N14:N15"/>
+    <mergeCell ref="O14:O15"/>
     <mergeCell ref="Q16:Q17"/>
     <mergeCell ref="R16:R17"/>
     <mergeCell ref="C23:C24"/>
@@ -3530,62 +3577,15 @@
     <mergeCell ref="N16:N17"/>
     <mergeCell ref="O16:O17"/>
     <mergeCell ref="P16:P17"/>
-    <mergeCell ref="P14:P15"/>
-    <mergeCell ref="Q14:Q15"/>
-    <mergeCell ref="R14:R15"/>
-    <mergeCell ref="D16:D17"/>
-    <mergeCell ref="E16:E17"/>
-    <mergeCell ref="F16:F17"/>
-    <mergeCell ref="G16:G17"/>
-    <mergeCell ref="H16:H17"/>
-    <mergeCell ref="I16:I17"/>
-    <mergeCell ref="J16:J17"/>
-    <mergeCell ref="J14:J15"/>
-    <mergeCell ref="K14:K15"/>
-    <mergeCell ref="L14:L15"/>
-    <mergeCell ref="M14:M15"/>
-    <mergeCell ref="N14:N15"/>
-    <mergeCell ref="O14:O15"/>
-    <mergeCell ref="R5:R6"/>
-    <mergeCell ref="R7:R8"/>
-    <mergeCell ref="C14:C15"/>
-    <mergeCell ref="C16:C17"/>
-    <mergeCell ref="D14:D15"/>
-    <mergeCell ref="E14:E15"/>
-    <mergeCell ref="F14:F15"/>
-    <mergeCell ref="G14:G15"/>
-    <mergeCell ref="H14:H15"/>
-    <mergeCell ref="I14:I15"/>
-    <mergeCell ref="O5:O6"/>
-    <mergeCell ref="O7:O8"/>
-    <mergeCell ref="P5:P6"/>
-    <mergeCell ref="P7:P8"/>
-    <mergeCell ref="Q5:Q6"/>
-    <mergeCell ref="Q7:Q8"/>
-    <mergeCell ref="L5:L6"/>
-    <mergeCell ref="L7:L8"/>
-    <mergeCell ref="M5:M6"/>
-    <mergeCell ref="M7:M8"/>
-    <mergeCell ref="N5:N6"/>
-    <mergeCell ref="N7:N8"/>
-    <mergeCell ref="I5:I6"/>
-    <mergeCell ref="I7:I8"/>
-    <mergeCell ref="J5:J6"/>
-    <mergeCell ref="J7:J8"/>
-    <mergeCell ref="K5:K6"/>
-    <mergeCell ref="K7:K8"/>
-    <mergeCell ref="F5:F6"/>
-    <mergeCell ref="F7:F8"/>
-    <mergeCell ref="G5:G6"/>
-    <mergeCell ref="G7:G8"/>
-    <mergeCell ref="H5:H6"/>
-    <mergeCell ref="H7:H8"/>
-    <mergeCell ref="C5:C6"/>
-    <mergeCell ref="C7:C8"/>
-    <mergeCell ref="D5:D6"/>
-    <mergeCell ref="D7:D8"/>
-    <mergeCell ref="E5:E6"/>
-    <mergeCell ref="E7:E8"/>
+    <mergeCell ref="P25:P26"/>
+    <mergeCell ref="Q25:Q26"/>
+    <mergeCell ref="R25:R26"/>
+    <mergeCell ref="J25:J26"/>
+    <mergeCell ref="K25:K26"/>
+    <mergeCell ref="L25:L26"/>
+    <mergeCell ref="M25:M26"/>
+    <mergeCell ref="N25:N26"/>
+    <mergeCell ref="O25:O26"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -3595,7 +3595,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6428E42B-41F2-4E3D-A8D3-BA9D08EC2A13}">
   <dimension ref="A1:Q23"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F25" sqref="F25"/>
     </sheetView>
   </sheetViews>
@@ -3661,37 +3661,37 @@
       <c r="A2" t="s">
         <v>32</v>
       </c>
-      <c r="B2" s="4">
+      <c r="B2" s="3">
         <v>0.41199999999999998</v>
       </c>
-      <c r="C2" s="4">
+      <c r="C2" s="3">
         <v>0.73</v>
       </c>
-      <c r="D2" s="4">
+      <c r="D2" s="3">
         <v>0.77500000000000002</v>
       </c>
-      <c r="E2" s="4">
+      <c r="E2" s="3">
         <v>0.78600000000000003</v>
       </c>
-      <c r="F2" s="4">
+      <c r="F2" s="3">
         <v>0.78800000000000003</v>
       </c>
-      <c r="G2" s="4">
+      <c r="G2" s="3">
         <v>0.69099999999999995</v>
       </c>
-      <c r="H2" s="4">
+      <c r="H2" s="3">
         <v>0.746</v>
       </c>
-      <c r="I2" s="4">
+      <c r="I2" s="3">
         <v>0.76300000000000001</v>
       </c>
-      <c r="J2" s="4">
+      <c r="J2" s="3">
         <v>0.76</v>
       </c>
-      <c r="K2" s="4">
+      <c r="K2" s="3">
         <v>0.75600000000000001</v>
       </c>
-      <c r="L2" s="4">
+      <c r="L2" s="3">
         <v>0.76300000000000001</v>
       </c>
       <c r="M2" s="2">
@@ -3700,13 +3700,13 @@
       <c r="N2" s="2">
         <v>0.79</v>
       </c>
-      <c r="O2" s="4">
+      <c r="O2" s="3">
         <v>0.8</v>
       </c>
-      <c r="P2" s="4">
+      <c r="P2" s="3">
         <v>0.76</v>
       </c>
-      <c r="Q2" s="4">
+      <c r="Q2" s="3">
         <v>0.73</v>
       </c>
     </row>
@@ -3714,37 +3714,37 @@
       <c r="A3" t="s">
         <v>33</v>
       </c>
-      <c r="B3" s="4">
+      <c r="B3" s="3">
         <v>6.5000000000000002E-2</v>
       </c>
-      <c r="C3" s="4">
+      <c r="C3" s="3">
         <v>0.20399999999999999</v>
       </c>
-      <c r="D3" s="4">
+      <c r="D3" s="3">
         <v>0.185</v>
       </c>
-      <c r="E3" s="4">
+      <c r="E3" s="3">
         <v>0.18099999999999999</v>
       </c>
-      <c r="F3" s="4">
+      <c r="F3" s="3">
         <v>0.183</v>
       </c>
-      <c r="G3" s="4">
+      <c r="G3" s="3">
         <v>0.254</v>
       </c>
-      <c r="H3" s="4">
+      <c r="H3" s="3">
         <v>0.214</v>
       </c>
-      <c r="I3" s="4">
+      <c r="I3" s="3">
         <v>0.19400000000000001</v>
       </c>
-      <c r="J3" s="4">
+      <c r="J3" s="3">
         <v>0.20499999999999999</v>
       </c>
-      <c r="K3" s="4">
+      <c r="K3" s="3">
         <v>0.221</v>
       </c>
-      <c r="L3" s="4">
+      <c r="L3" s="3">
         <v>0.216</v>
       </c>
       <c r="M3" s="2">
@@ -3753,13 +3753,13 @@
       <c r="N3" s="2">
         <v>0.2</v>
       </c>
-      <c r="O3" s="4">
+      <c r="O3" s="3">
         <v>0.17100000000000001</v>
       </c>
-      <c r="P3" s="4">
+      <c r="P3" s="3">
         <v>0.15</v>
       </c>
-      <c r="Q3" s="4">
+      <c r="Q3" s="3">
         <v>0.12</v>
       </c>
     </row>
@@ -3767,52 +3767,52 @@
       <c r="A4" t="s">
         <v>34</v>
       </c>
-      <c r="B4" s="4">
+      <c r="B4" s="3">
         <v>8.0000000000000002E-3</v>
       </c>
-      <c r="C4" s="4">
+      <c r="C4" s="3">
         <v>1.0999999999999999E-2</v>
       </c>
-      <c r="D4" s="4">
+      <c r="D4" s="3">
         <v>8.9999999999999993E-3</v>
       </c>
-      <c r="E4" s="4">
+      <c r="E4" s="3">
         <v>1.2999999999999999E-2</v>
       </c>
-      <c r="F4" s="4">
+      <c r="F4" s="3">
         <v>8.9999999999999993E-3</v>
       </c>
-      <c r="G4" s="4">
+      <c r="G4" s="3">
         <v>8.9999999999999993E-3</v>
       </c>
-      <c r="H4" s="4">
+      <c r="H4" s="3">
         <v>7.0000000000000001E-3</v>
       </c>
-      <c r="I4" s="4">
+      <c r="I4" s="3">
         <v>0.01</v>
       </c>
-      <c r="J4" s="4">
+      <c r="J4" s="3">
         <v>8.9999999999999993E-3</v>
       </c>
-      <c r="K4" s="4">
+      <c r="K4" s="3">
         <v>1.2999999999999999E-2</v>
       </c>
-      <c r="L4" s="4">
+      <c r="L4" s="3">
         <v>1.4E-2</v>
       </c>
-      <c r="M4" s="4">
+      <c r="M4" s="3">
         <v>1.2E-2</v>
       </c>
       <c r="N4" s="2">
         <v>0.01</v>
       </c>
-      <c r="O4" s="4">
+      <c r="O4" s="3">
         <v>1.2999999999999999E-2</v>
       </c>
-      <c r="P4" s="4">
+      <c r="P4" s="3">
         <v>4.0000000000000001E-3</v>
       </c>
-      <c r="Q4" s="4">
+      <c r="Q4" s="3">
         <v>0.01</v>
       </c>
     </row>
@@ -3820,31 +3820,31 @@
       <c r="A5" t="s">
         <v>35</v>
       </c>
-      <c r="B5" s="4">
+      <c r="B5" s="3">
         <v>0.01</v>
       </c>
-      <c r="C5" s="4">
+      <c r="C5" s="3">
         <v>3.5000000000000003E-2</v>
       </c>
-      <c r="D5" s="4">
+      <c r="D5" s="3">
         <v>1.2999999999999999E-2</v>
       </c>
-      <c r="E5" s="4">
+      <c r="E5" s="3">
         <v>8.0000000000000002E-3</v>
       </c>
-      <c r="F5" s="4">
+      <c r="F5" s="3">
         <v>6.0000000000000001E-3</v>
       </c>
-      <c r="G5" s="4">
+      <c r="G5" s="3">
         <v>2.9000000000000001E-2</v>
       </c>
-      <c r="H5" s="4">
+      <c r="H5" s="3">
         <v>1.0999999999999999E-2</v>
       </c>
-      <c r="I5" s="4">
+      <c r="I5" s="3">
         <v>2.3E-2</v>
       </c>
-      <c r="J5" s="4">
+      <c r="J5" s="3">
         <v>2.3E-2</v>
       </c>
       <c r="K5" t="s">
@@ -3873,22 +3873,22 @@
       <c r="A6" t="s">
         <v>36</v>
       </c>
-      <c r="B6" s="4">
-        <v>0</v>
-      </c>
-      <c r="C6" s="4">
+      <c r="B6" s="3">
+        <v>0</v>
+      </c>
+      <c r="C6" s="3">
         <v>0.02</v>
       </c>
-      <c r="D6" s="4">
+      <c r="D6" s="3">
         <v>1.7999999999999999E-2</v>
       </c>
-      <c r="E6" s="4">
+      <c r="E6" s="3">
         <v>1.2E-2</v>
       </c>
-      <c r="F6" s="4">
+      <c r="F6" s="3">
         <v>1.2999999999999999E-2</v>
       </c>
-      <c r="G6" s="4">
+      <c r="G6" s="3">
         <v>1.7000000000000001E-2</v>
       </c>
       <c r="H6" t="s">
@@ -3926,37 +3926,37 @@
       <c r="A7" t="s">
         <v>37</v>
       </c>
-      <c r="B7" s="4">
+      <c r="B7" s="3">
         <v>0.505</v>
       </c>
-      <c r="C7" s="4">
+      <c r="C7" s="3">
         <v>0.13200000000000001</v>
       </c>
-      <c r="D7" s="4">
+      <c r="D7" s="3">
         <v>0.115</v>
       </c>
-      <c r="E7" s="4">
+      <c r="E7" s="3">
         <v>0.123</v>
       </c>
-      <c r="F7" s="4">
+      <c r="F7" s="3">
         <v>0.108</v>
       </c>
-      <c r="G7" s="4">
+      <c r="G7" s="3">
         <v>0.11</v>
       </c>
-      <c r="H7" s="4">
+      <c r="H7" s="3">
         <v>9.9000000000000005E-2</v>
       </c>
-      <c r="I7" s="4">
+      <c r="I7" s="3">
         <v>9.5000000000000001E-2</v>
       </c>
-      <c r="J7" s="4">
+      <c r="J7" s="3">
         <v>0.10100000000000001</v>
       </c>
-      <c r="K7" s="4">
+      <c r="K7" s="3">
         <v>9.2999999999999999E-2</v>
       </c>
-      <c r="L7" s="4">
+      <c r="L7" s="3">
         <v>0.1</v>
       </c>
       <c r="M7" s="2">
@@ -3965,13 +3965,13 @@
       <c r="N7" s="2">
         <v>0.1</v>
       </c>
-      <c r="O7" s="4">
+      <c r="O7" s="3">
         <v>0.12</v>
       </c>
-      <c r="P7" s="4">
+      <c r="P7" s="3">
         <v>0.06</v>
       </c>
-      <c r="Q7" s="4">
+      <c r="Q7" s="3">
         <v>0.08</v>
       </c>
     </row>
@@ -4032,37 +4032,37 @@
       <c r="A10" t="s">
         <v>32</v>
       </c>
-      <c r="B10" s="4">
+      <c r="B10" s="3">
         <v>0.65600000000000003</v>
       </c>
-      <c r="C10" s="4">
+      <c r="C10" s="3">
         <v>0.81799999999999995</v>
       </c>
-      <c r="D10" s="4">
+      <c r="D10" s="3">
         <v>0.64200000000000002</v>
       </c>
-      <c r="E10" s="4">
+      <c r="E10" s="3">
         <v>0.72799999999999998</v>
       </c>
-      <c r="F10" s="4">
+      <c r="F10" s="3">
         <v>0.73599999999999999</v>
       </c>
-      <c r="G10" s="4">
+      <c r="G10" s="3">
         <v>0.73499999999999999</v>
       </c>
-      <c r="H10" s="4">
+      <c r="H10" s="3">
         <v>0.75900000000000001</v>
       </c>
-      <c r="I10" s="4">
+      <c r="I10" s="3">
         <v>0.71799999999999997</v>
       </c>
-      <c r="J10" s="4">
+      <c r="J10" s="3">
         <v>0.72099999999999997</v>
       </c>
-      <c r="K10" s="4">
+      <c r="K10" s="3">
         <v>0.73799999999999999</v>
       </c>
-      <c r="L10" s="4">
+      <c r="L10" s="3">
         <v>0.73299999999999998</v>
       </c>
       <c r="M10" t="s">
@@ -4085,37 +4085,37 @@
       <c r="A11" t="s">
         <v>33</v>
       </c>
-      <c r="B11" s="4">
+      <c r="B11" s="3">
         <v>0.214</v>
       </c>
-      <c r="C11" s="4">
+      <c r="C11" s="3">
         <v>0.17699999999999999</v>
       </c>
-      <c r="D11" s="4">
+      <c r="D11" s="3">
         <v>0.27600000000000002</v>
       </c>
-      <c r="E11" s="4">
+      <c r="E11" s="3">
         <v>0.254</v>
       </c>
-      <c r="F11" s="4">
+      <c r="F11" s="3">
         <v>0.23400000000000001</v>
       </c>
-      <c r="G11" s="4">
+      <c r="G11" s="3">
         <v>0.22500000000000001</v>
       </c>
-      <c r="H11" s="4">
+      <c r="H11" s="3">
         <v>0.23100000000000001</v>
       </c>
-      <c r="I11" s="4">
+      <c r="I11" s="3">
         <v>0.26</v>
       </c>
-      <c r="J11" s="4">
+      <c r="J11" s="3">
         <v>0.23100000000000001</v>
       </c>
-      <c r="K11" s="4">
+      <c r="K11" s="3">
         <v>0.23899999999999999</v>
       </c>
-      <c r="L11" s="4">
+      <c r="L11" s="3">
         <v>0.249</v>
       </c>
       <c r="M11" t="s">
@@ -4138,43 +4138,43 @@
       <c r="A12" t="s">
         <v>34</v>
       </c>
-      <c r="B12" s="4">
+      <c r="B12" s="3">
         <v>7.0000000000000001E-3</v>
       </c>
-      <c r="C12" s="4">
+      <c r="C12" s="3">
         <v>3.0000000000000001E-3</v>
       </c>
-      <c r="D12" s="4">
+      <c r="D12" s="3">
         <v>1.6E-2</v>
       </c>
-      <c r="E12" s="4">
+      <c r="E12" s="3">
         <v>7.0000000000000001E-3</v>
       </c>
-      <c r="F12" s="4">
+      <c r="F12" s="3">
         <v>8.9999999999999993E-3</v>
       </c>
-      <c r="G12" s="4">
+      <c r="G12" s="3">
         <v>7.0000000000000001E-3</v>
       </c>
-      <c r="H12" s="4">
+      <c r="H12" s="3">
         <v>6.0000000000000001E-3</v>
       </c>
-      <c r="I12" s="4">
+      <c r="I12" s="3">
         <v>2E-3</v>
       </c>
-      <c r="J12" s="4">
+      <c r="J12" s="3">
         <v>4.0000000000000001E-3</v>
       </c>
-      <c r="K12" s="4">
+      <c r="K12" s="3">
         <v>5.0000000000000001E-3</v>
       </c>
-      <c r="L12" s="4">
+      <c r="L12" s="3">
         <v>3.0000000000000001E-3</v>
       </c>
       <c r="M12" t="s">
         <v>0</v>
       </c>
-      <c r="N12" s="4">
+      <c r="N12" s="3">
         <v>5.0000000000000001E-3</v>
       </c>
       <c r="O12" s="2">
@@ -4191,31 +4191,31 @@
       <c r="A13" t="s">
         <v>35</v>
       </c>
-      <c r="B13" s="4">
+      <c r="B13" s="3">
         <v>2E-3</v>
       </c>
-      <c r="C13" s="4">
+      <c r="C13" s="3">
         <v>2E-3</v>
       </c>
-      <c r="D13" s="4">
+      <c r="D13" s="3">
         <v>4.8000000000000001E-2</v>
       </c>
-      <c r="E13" s="4">
+      <c r="E13" s="3">
         <v>4.0000000000000001E-3</v>
       </c>
-      <c r="F13" s="4">
+      <c r="F13" s="3">
         <v>6.0000000000000001E-3</v>
       </c>
-      <c r="G13" s="4">
+      <c r="G13" s="3">
         <v>1.7999999999999999E-2</v>
       </c>
-      <c r="H13" s="4">
+      <c r="H13" s="3">
         <v>4.0000000000000001E-3</v>
       </c>
-      <c r="I13" s="4">
+      <c r="I13" s="3">
         <v>1.2999999999999999E-2</v>
       </c>
-      <c r="J13" s="4">
+      <c r="J13" s="3">
         <v>3.3000000000000002E-2</v>
       </c>
       <c r="K13" t="s">
@@ -4244,22 +4244,22 @@
       <c r="A14" t="s">
         <v>36</v>
       </c>
-      <c r="B14" s="4">
-        <v>0</v>
-      </c>
-      <c r="C14" s="4">
-        <v>0</v>
-      </c>
-      <c r="D14" s="4">
+      <c r="B14" s="3">
+        <v>0</v>
+      </c>
+      <c r="C14" s="3">
+        <v>0</v>
+      </c>
+      <c r="D14" s="3">
         <v>1.7999999999999999E-2</v>
       </c>
-      <c r="E14" s="4">
+      <c r="E14" s="3">
         <v>7.0000000000000001E-3</v>
       </c>
-      <c r="F14" s="4">
+      <c r="F14" s="3">
         <v>1.4E-2</v>
       </c>
-      <c r="G14" s="4">
+      <c r="G14" s="3">
         <v>1.4999999999999999E-2</v>
       </c>
       <c r="H14" t="s">
@@ -4297,43 +4297,43 @@
       <c r="A15" t="s">
         <v>37</v>
       </c>
-      <c r="B15" s="4">
+      <c r="B15" s="3">
         <v>0.121</v>
       </c>
-      <c r="C15" s="4">
+      <c r="C15" s="3">
         <v>7.5999999999999998E-2</v>
       </c>
-      <c r="D15" s="4">
+      <c r="D15" s="3">
         <v>0.14000000000000001</v>
       </c>
-      <c r="E15" s="4">
+      <c r="E15" s="3">
         <v>9.1999999999999998E-2</v>
       </c>
-      <c r="F15" s="4">
+      <c r="F15" s="3">
         <v>0.10199999999999999</v>
       </c>
-      <c r="G15" s="4">
+      <c r="G15" s="3">
         <v>0.11</v>
       </c>
-      <c r="H15" s="4">
+      <c r="H15" s="3">
         <v>6.0999999999999999E-2</v>
       </c>
-      <c r="I15" s="4">
+      <c r="I15" s="3">
         <v>0.128</v>
       </c>
-      <c r="J15" s="4">
+      <c r="J15" s="3">
         <v>0.109</v>
       </c>
-      <c r="K15" s="4">
+      <c r="K15" s="3">
         <v>9.1999999999999998E-2</v>
       </c>
-      <c r="L15" s="4">
+      <c r="L15" s="3">
         <v>6.0999999999999999E-2</v>
       </c>
       <c r="M15" t="s">
         <v>0</v>
       </c>
-      <c r="N15" s="4">
+      <c r="N15" s="3">
         <v>7.1999999999999995E-2</v>
       </c>
       <c r="O15" s="2">
@@ -4403,37 +4403,37 @@
       <c r="A18" t="s">
         <v>32</v>
       </c>
-      <c r="B18" s="4">
+      <c r="B18" s="3">
         <v>0.45100000000000001</v>
       </c>
-      <c r="C18" s="4">
+      <c r="C18" s="3">
         <v>0.75900000000000001</v>
       </c>
-      <c r="D18" s="4">
+      <c r="D18" s="3">
         <v>0.75</v>
       </c>
-      <c r="E18" s="4">
+      <c r="E18" s="3">
         <v>0.77</v>
       </c>
-      <c r="F18" s="4">
+      <c r="F18" s="3">
         <v>0.77400000000000002</v>
       </c>
-      <c r="G18" s="4">
+      <c r="G18" s="3">
         <v>0.70499999999999996</v>
       </c>
-      <c r="H18" s="4">
+      <c r="H18" s="3">
         <v>0.75</v>
       </c>
-      <c r="I18" s="4">
+      <c r="I18" s="3">
         <v>0.75</v>
       </c>
-      <c r="J18" s="4">
+      <c r="J18" s="3">
         <v>0.745</v>
       </c>
-      <c r="K18" s="4">
+      <c r="K18" s="3">
         <v>0.752</v>
       </c>
-      <c r="L18" s="4">
+      <c r="L18" s="3">
         <v>0.75600000000000001</v>
       </c>
       <c r="M18" t="s">
@@ -4442,13 +4442,13 @@
       <c r="N18" s="2">
         <v>0.78</v>
       </c>
-      <c r="O18" s="4">
+      <c r="O18" s="3">
         <v>0.79200000000000004</v>
       </c>
-      <c r="P18" s="4">
+      <c r="P18" s="3">
         <v>0.75</v>
       </c>
-      <c r="Q18" s="4">
+      <c r="Q18" s="3">
         <v>0.73</v>
       </c>
     </row>
@@ -4456,37 +4456,37 @@
       <c r="A19" t="s">
         <v>33</v>
       </c>
-      <c r="B19" s="4">
+      <c r="B19" s="3">
         <v>8.8999999999999996E-2</v>
       </c>
-      <c r="C19" s="4">
+      <c r="C19" s="3">
         <v>0.19500000000000001</v>
       </c>
-      <c r="D19" s="4">
+      <c r="D19" s="3">
         <v>0.20200000000000001</v>
       </c>
-      <c r="E19" s="4">
+      <c r="E19" s="3">
         <v>0.20200000000000001</v>
       </c>
-      <c r="F19" s="4">
+      <c r="F19" s="3">
         <v>0.19700000000000001</v>
       </c>
-      <c r="G19" s="4">
+      <c r="G19" s="3">
         <v>0.245</v>
       </c>
-      <c r="H19" s="4">
+      <c r="H19" s="3">
         <v>0.22</v>
       </c>
-      <c r="I19" s="4">
+      <c r="I19" s="3">
         <v>0.21299999999999999</v>
       </c>
-      <c r="J19" s="4">
+      <c r="J19" s="3">
         <v>0.21299999999999999</v>
       </c>
-      <c r="K19" s="4">
+      <c r="K19" s="3">
         <v>0.22500000000000001</v>
       </c>
-      <c r="L19" s="4">
+      <c r="L19" s="3">
         <v>0.223</v>
       </c>
       <c r="M19" t="s">
@@ -4495,13 +4495,13 @@
       <c r="N19" s="2">
         <v>0.2</v>
       </c>
-      <c r="O19" s="4">
+      <c r="O19" s="3">
         <v>0.18</v>
       </c>
-      <c r="P19" s="4">
+      <c r="P19" s="3">
         <v>0.16</v>
       </c>
-      <c r="Q19" s="4">
+      <c r="Q19" s="3">
         <v>0.14000000000000001</v>
       </c>
     </row>
@@ -4509,52 +4509,52 @@
       <c r="A20" t="s">
         <v>34</v>
       </c>
-      <c r="B20" s="4">
+      <c r="B20" s="3">
         <v>8.0000000000000002E-3</v>
       </c>
-      <c r="C20" s="4">
+      <c r="C20" s="3">
         <v>8.0000000000000002E-3</v>
       </c>
-      <c r="D20" s="4">
+      <c r="D20" s="3">
         <v>0.01</v>
       </c>
-      <c r="E20" s="4">
+      <c r="E20" s="3">
         <v>1.0999999999999999E-2</v>
       </c>
-      <c r="F20" s="4">
+      <c r="F20" s="3">
         <v>8.9999999999999993E-3</v>
       </c>
-      <c r="G20" s="4">
+      <c r="G20" s="3">
         <v>8.0000000000000002E-3</v>
       </c>
-      <c r="H20" s="4">
+      <c r="H20" s="3">
         <v>7.0000000000000001E-3</v>
       </c>
-      <c r="I20" s="4">
+      <c r="I20" s="3">
         <v>8.0000000000000002E-3</v>
       </c>
-      <c r="J20" s="4">
+      <c r="J20" s="3">
         <v>7.0000000000000001E-3</v>
       </c>
-      <c r="K20" s="4">
+      <c r="K20" s="3">
         <v>1.0999999999999999E-2</v>
       </c>
-      <c r="L20" s="4">
+      <c r="L20" s="3">
         <v>1.0999999999999999E-2</v>
       </c>
       <c r="M20" t="s">
         <v>0</v>
       </c>
-      <c r="N20" s="4">
+      <c r="N20" s="3">
         <v>1.0999999999999999E-2</v>
       </c>
-      <c r="O20" s="4">
+      <c r="O20" s="3">
         <v>1.2E-2</v>
       </c>
-      <c r="P20" s="4">
+      <c r="P20" s="3">
         <v>4.0000000000000001E-3</v>
       </c>
-      <c r="Q20" s="4">
+      <c r="Q20" s="3">
         <v>6.0000000000000001E-3</v>
       </c>
     </row>
@@ -4562,31 +4562,31 @@
       <c r="A21" t="s">
         <v>35</v>
       </c>
-      <c r="B21" s="4">
+      <c r="B21" s="3">
         <v>8.9999999999999993E-3</v>
       </c>
-      <c r="C21" s="4">
+      <c r="C21" s="3">
         <v>2.5000000000000001E-2</v>
       </c>
-      <c r="D21" s="4">
+      <c r="D21" s="3">
         <v>0.02</v>
       </c>
-      <c r="E21" s="4">
+      <c r="E21" s="3">
         <v>7.0000000000000001E-3</v>
       </c>
-      <c r="F21" s="4">
+      <c r="F21" s="3">
         <v>6.0000000000000001E-3</v>
       </c>
-      <c r="G21" s="4">
+      <c r="G21" s="3">
         <v>2.5999999999999999E-2</v>
       </c>
-      <c r="H21" s="4">
+      <c r="H21" s="3">
         <v>8.0000000000000002E-3</v>
       </c>
-      <c r="I21" s="4">
+      <c r="I21" s="3">
         <v>0.02</v>
       </c>
-      <c r="J21" s="4">
+      <c r="J21" s="3">
         <v>2.7E-2</v>
       </c>
       <c r="K21" t="s">
@@ -4615,31 +4615,31 @@
       <c r="A22" t="s">
         <v>36</v>
       </c>
-      <c r="B22" s="4">
+      <c r="B22" s="3">
         <v>8.9999999999999993E-3</v>
       </c>
-      <c r="C22" s="4">
+      <c r="C22" s="3">
         <v>2.5000000000000001E-2</v>
       </c>
-      <c r="D22" s="4">
+      <c r="D22" s="3">
         <v>0.02</v>
       </c>
-      <c r="E22" s="4">
+      <c r="E22" s="3">
         <v>7.0000000000000001E-3</v>
       </c>
-      <c r="F22" s="4">
+      <c r="F22" s="3">
         <v>6.0000000000000001E-3</v>
       </c>
-      <c r="G22" s="4">
+      <c r="G22" s="3">
         <v>2.5999999999999999E-2</v>
       </c>
-      <c r="H22" s="4">
+      <c r="H22" s="3">
         <v>8.0000000000000002E-3</v>
       </c>
-      <c r="I22" s="4">
+      <c r="I22" s="3">
         <v>0.02</v>
       </c>
-      <c r="J22" s="4">
+      <c r="J22" s="3">
         <v>2.7E-2</v>
       </c>
       <c r="K22" t="s">
@@ -4668,43 +4668,43 @@
       <c r="A23" t="s">
         <v>37</v>
       </c>
-      <c r="B23" s="4">
+      <c r="B23" s="3">
         <v>0.443</v>
       </c>
-      <c r="C23" s="4">
+      <c r="C23" s="3">
         <v>0.114</v>
       </c>
-      <c r="D23" s="4">
+      <c r="D23" s="3">
         <v>0.12</v>
       </c>
-      <c r="E23" s="4">
+      <c r="E23" s="3">
         <v>0.114</v>
       </c>
-      <c r="F23" s="4">
+      <c r="F23" s="3">
         <v>0.10199999999999999</v>
       </c>
-      <c r="G23" s="4">
+      <c r="G23" s="3">
         <v>0.11</v>
       </c>
-      <c r="H23" s="4">
+      <c r="H23" s="3">
         <v>8.5999999999999993E-2</v>
       </c>
-      <c r="I23" s="4">
+      <c r="I23" s="3">
         <v>0.105</v>
       </c>
-      <c r="J23" s="4">
+      <c r="J23" s="3">
         <v>0.104</v>
       </c>
-      <c r="K23" s="4">
+      <c r="K23" s="3">
         <v>0.1</v>
       </c>
-      <c r="L23" s="4">
+      <c r="L23" s="3">
         <v>9.0999999999999998E-2</v>
       </c>
       <c r="M23" t="s">
         <v>0</v>
       </c>
-      <c r="N23" s="4">
+      <c r="N23" s="3">
         <v>0.10199999999999999</v>
       </c>
       <c r="O23" s="2">
@@ -4726,25 +4726,25 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BF6AA138-D3EB-4C18-9B6B-D096DF1028EC}">
   <dimension ref="A1:G19"/>
   <sheetViews>
-    <sheetView topLeftCell="A6" workbookViewId="0">
+    <sheetView topLeftCell="A3" workbookViewId="0">
       <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="C1" s="3"/>
-      <c r="D1" s="3" t="s">
+      <c r="C1" s="5"/>
+      <c r="D1" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="E1" s="3"/>
-      <c r="F1" s="3" t="s">
+      <c r="E1" s="5"/>
+      <c r="F1" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="G1" s="3"/>
+      <c r="G1" s="5"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
@@ -4776,19 +4776,19 @@
       <c r="B3">
         <v>202</v>
       </c>
-      <c r="C3" s="4">
+      <c r="C3" s="3">
         <v>-5.0000000000000001E-3</v>
       </c>
       <c r="D3">
         <v>115</v>
       </c>
-      <c r="E3" s="4">
+      <c r="E3" s="3">
         <v>-3.3000000000000002E-2</v>
       </c>
       <c r="F3">
         <v>317</v>
       </c>
-      <c r="G3" s="4">
+      <c r="G3" s="3">
         <v>-1.6E-2</v>
       </c>
     </row>
@@ -4799,19 +4799,19 @@
       <c r="B4">
         <v>203</v>
       </c>
-      <c r="C4" s="4">
+      <c r="C4" s="3">
         <v>0.187</v>
       </c>
       <c r="D4">
         <v>119</v>
       </c>
-      <c r="E4" s="4">
+      <c r="E4" s="3">
         <v>9.4E-2</v>
       </c>
       <c r="F4">
         <v>322</v>
       </c>
-      <c r="G4" s="4">
+      <c r="G4" s="3">
         <v>8.3000000000000004E-2</v>
       </c>
     </row>
@@ -4822,19 +4822,19 @@
       <c r="B5">
         <v>171</v>
       </c>
-      <c r="C5" s="4">
+      <c r="C5" s="3">
         <v>-0.40200000000000002</v>
       </c>
       <c r="D5">
         <v>77</v>
       </c>
-      <c r="E5" s="4">
+      <c r="E5" s="3">
         <v>5.2999999999999999E-2</v>
       </c>
       <c r="F5">
         <v>248</v>
       </c>
-      <c r="G5" s="4">
+      <c r="G5" s="3">
         <v>5.5E-2</v>
       </c>
     </row>
@@ -4845,19 +4845,19 @@
       <c r="B6">
         <v>286</v>
       </c>
-      <c r="C6" s="4">
+      <c r="C6" s="3">
         <v>2.5000000000000001E-2</v>
       </c>
       <c r="D6">
         <v>201</v>
       </c>
-      <c r="E6" s="4">
+      <c r="E6" s="3">
         <v>0.13300000000000001</v>
       </c>
       <c r="F6">
         <v>487</v>
       </c>
-      <c r="G6" s="4">
+      <c r="G6" s="3">
         <v>0.114</v>
       </c>
     </row>
@@ -4868,19 +4868,19 @@
       <c r="B7">
         <v>279</v>
       </c>
-      <c r="C7" s="4">
+      <c r="C7" s="3">
         <v>-5.7000000000000002E-2</v>
       </c>
       <c r="D7">
         <v>120</v>
       </c>
-      <c r="E7" s="4">
+      <c r="E7" s="3">
         <v>0.11899999999999999</v>
       </c>
       <c r="F7">
         <v>399</v>
       </c>
-      <c r="G7" s="4">
+      <c r="G7" s="3">
         <v>0.106</v>
       </c>
     </row>
@@ -4891,19 +4891,19 @@
       <c r="B8">
         <v>296</v>
       </c>
-      <c r="C8" s="4">
+      <c r="C8" s="3">
         <v>-2.5999999999999999E-2</v>
       </c>
       <c r="D8">
         <v>198</v>
       </c>
-      <c r="E8" s="4">
+      <c r="E8" s="3">
         <v>0.14599999999999999</v>
       </c>
       <c r="F8">
         <v>494</v>
       </c>
-      <c r="G8" s="4">
+      <c r="G8" s="3">
         <v>0.11700000000000001</v>
       </c>
     </row>
@@ -4914,19 +4914,19 @@
       <c r="B9">
         <v>304</v>
       </c>
-      <c r="C9" s="4">
+      <c r="C9" s="3">
         <v>-0.23799999999999999</v>
       </c>
       <c r="D9">
         <v>245</v>
       </c>
-      <c r="E9" s="4">
+      <c r="E9" s="3">
         <v>0.157</v>
       </c>
       <c r="F9">
         <v>549</v>
       </c>
-      <c r="G9" s="4">
+      <c r="G9" s="3">
         <v>0.122</v>
       </c>
     </row>
@@ -4937,19 +4937,19 @@
       <c r="B10">
         <v>399</v>
       </c>
-      <c r="C10" s="4">
+      <c r="C10" s="3">
         <v>0.153</v>
       </c>
       <c r="D10">
         <v>202</v>
       </c>
-      <c r="E10" s="4">
+      <c r="E10" s="3">
         <v>0.16400000000000001</v>
       </c>
       <c r="F10">
         <v>601</v>
       </c>
-      <c r="G10" s="4">
+      <c r="G10" s="3">
         <v>0.13200000000000001</v>
       </c>
     </row>
@@ -4960,19 +4960,19 @@
       <c r="B11">
         <v>346</v>
       </c>
-      <c r="C11" s="4">
+      <c r="C11" s="3">
         <v>-0.25600000000000001</v>
       </c>
       <c r="D11">
         <v>406</v>
       </c>
-      <c r="E11" s="4">
+      <c r="E11" s="3">
         <v>0.192</v>
       </c>
       <c r="F11">
         <v>752</v>
       </c>
-      <c r="G11" s="4">
+      <c r="G11" s="3">
         <v>0.14899999999999999</v>
       </c>
     </row>
@@ -4983,19 +4983,19 @@
       <c r="B12">
         <v>465</v>
       </c>
-      <c r="C12" s="4">
+      <c r="C12" s="3">
         <v>0.14499999999999999</v>
       </c>
       <c r="D12">
         <v>256</v>
       </c>
-      <c r="E12" s="4">
+      <c r="E12" s="3">
         <v>0.26800000000000002</v>
       </c>
       <c r="F12">
         <v>721</v>
       </c>
-      <c r="G12" s="4">
+      <c r="G12" s="3">
         <v>0.16</v>
       </c>
     </row>
@@ -5006,19 +5006,19 @@
       <c r="B13">
         <v>406</v>
       </c>
-      <c r="C13" s="4">
+      <c r="C13" s="3">
         <v>0.504</v>
       </c>
       <c r="D13">
         <v>306</v>
       </c>
-      <c r="E13" s="4">
+      <c r="E13" s="3">
         <v>0.255</v>
       </c>
       <c r="F13">
         <v>712</v>
       </c>
-      <c r="G13" s="4">
+      <c r="G13" s="3">
         <v>0.155</v>
       </c>
     </row>
@@ -5029,7 +5029,7 @@
       <c r="B14">
         <v>270</v>
       </c>
-      <c r="C14" s="4">
+      <c r="C14" s="3">
         <v>0.08</v>
       </c>
       <c r="D14" t="s">
@@ -5052,19 +5052,19 @@
       <c r="B15">
         <v>250</v>
       </c>
-      <c r="C15" s="4">
+      <c r="C15" s="3">
         <v>3.3000000000000002E-2</v>
       </c>
       <c r="D15">
         <v>250</v>
       </c>
-      <c r="E15" s="4">
+      <c r="E15" s="3">
         <v>0.151</v>
       </c>
       <c r="F15">
         <v>500</v>
       </c>
-      <c r="G15" s="4">
+      <c r="G15" s="3">
         <v>0.10100000000000001</v>
       </c>
     </row>
@@ -5081,13 +5081,13 @@
       <c r="D16">
         <v>115</v>
       </c>
-      <c r="E16" s="4">
+      <c r="E16" s="3">
         <v>0.14099999999999999</v>
       </c>
       <c r="F16">
         <v>357</v>
       </c>
-      <c r="G16" s="4">
+      <c r="G16" s="3">
         <v>9.1999999999999998E-2</v>
       </c>
     </row>
@@ -5104,13 +5104,13 @@
       <c r="D17" t="s">
         <v>0</v>
       </c>
-      <c r="E17" s="4">
+      <c r="E17" s="3">
         <v>0.184</v>
       </c>
       <c r="F17" t="s">
         <v>0</v>
       </c>
-      <c r="G17" s="4">
+      <c r="G17" s="3">
         <v>0.154</v>
       </c>
     </row>
@@ -5195,7 +5195,7 @@
       <c r="A2" t="s">
         <v>45</v>
       </c>
-      <c r="B2" s="4">
+      <c r="B2" s="3">
         <v>0.46899999999999997</v>
       </c>
     </row>
@@ -5203,7 +5203,7 @@
       <c r="A3" t="s">
         <v>46</v>
       </c>
-      <c r="B3" s="4">
+      <c r="B3" s="3">
         <v>0.185</v>
       </c>
     </row>
@@ -5211,7 +5211,7 @@
       <c r="A4" t="s">
         <v>47</v>
       </c>
-      <c r="B4" s="4">
+      <c r="B4" s="3">
         <v>0.14799999999999999</v>
       </c>
     </row>
@@ -5219,7 +5219,7 @@
       <c r="A5" t="s">
         <v>48</v>
       </c>
-      <c r="B5" s="4">
+      <c r="B5" s="3">
         <v>9.9000000000000005E-2</v>
       </c>
     </row>
@@ -5227,7 +5227,7 @@
       <c r="A6" t="s">
         <v>49</v>
       </c>
-      <c r="B6" s="4">
+      <c r="B6" s="3">
         <v>6.2E-2</v>
       </c>
     </row>
@@ -5235,7 +5235,7 @@
       <c r="A7" t="s">
         <v>50</v>
       </c>
-      <c r="B7" s="4">
+      <c r="B7" s="3">
         <v>1.2E-2</v>
       </c>
     </row>
@@ -5243,7 +5243,7 @@
       <c r="A8" t="s">
         <v>51</v>
       </c>
-      <c r="B8" s="4">
+      <c r="B8" s="3">
         <v>2.5000000000000001E-2</v>
       </c>
     </row>
@@ -5251,7 +5251,7 @@
       <c r="A9" t="s">
         <v>18</v>
       </c>
-      <c r="B9" s="4">
+      <c r="B9" s="3">
         <v>1</v>
       </c>
     </row>
@@ -5264,13 +5264,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{809DC106-1DD9-493E-9C70-484C3810AA18}">
   <dimension ref="A1:C16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="35.36328125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.08984375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.35">
@@ -5291,7 +5292,7 @@
       <c r="B2">
         <v>170</v>
       </c>
-      <c r="C2" s="4">
+      <c r="C2" s="3">
         <v>0.2</v>
       </c>
     </row>
@@ -5302,7 +5303,7 @@
       <c r="B3">
         <v>125</v>
       </c>
-      <c r="C3" s="4">
+      <c r="C3" s="3">
         <v>0.14699999999999999</v>
       </c>
     </row>
@@ -5313,7 +5314,7 @@
       <c r="B4">
         <v>118</v>
       </c>
-      <c r="C4" s="4">
+      <c r="C4" s="3">
         <v>0.13900000000000001</v>
       </c>
     </row>
@@ -5324,7 +5325,7 @@
       <c r="B5">
         <v>112</v>
       </c>
-      <c r="C5" s="4">
+      <c r="C5" s="3">
         <v>0.13200000000000001</v>
       </c>
     </row>
@@ -5335,7 +5336,7 @@
       <c r="B6">
         <v>71</v>
       </c>
-      <c r="C6" s="4">
+      <c r="C6" s="3">
         <v>8.4000000000000005E-2</v>
       </c>
     </row>
@@ -5346,7 +5347,7 @@
       <c r="B7">
         <v>58</v>
       </c>
-      <c r="C7" s="4">
+      <c r="C7" s="3">
         <v>6.8000000000000005E-2</v>
       </c>
     </row>
@@ -5357,7 +5358,7 @@
       <c r="B8">
         <v>54</v>
       </c>
-      <c r="C8" s="4">
+      <c r="C8" s="3">
         <v>6.4000000000000001E-2</v>
       </c>
     </row>
@@ -5368,7 +5369,7 @@
       <c r="B9">
         <v>38</v>
       </c>
-      <c r="C9" s="4">
+      <c r="C9" s="3">
         <v>4.4999999999999998E-2</v>
       </c>
     </row>
@@ -5379,7 +5380,7 @@
       <c r="B10">
         <v>33</v>
       </c>
-      <c r="C10" s="4">
+      <c r="C10" s="3">
         <v>3.9E-2</v>
       </c>
     </row>
@@ -5390,7 +5391,7 @@
       <c r="B11">
         <v>29</v>
       </c>
-      <c r="C11" s="4">
+      <c r="C11" s="3">
         <v>3.4000000000000002E-2</v>
       </c>
     </row>
@@ -5401,7 +5402,7 @@
       <c r="B12">
         <v>13</v>
       </c>
-      <c r="C12" s="4">
+      <c r="C12" s="3">
         <v>1.4999999999999999E-2</v>
       </c>
     </row>
@@ -5412,7 +5413,7 @@
       <c r="B13">
         <v>13</v>
       </c>
-      <c r="C13" s="4">
+      <c r="C13" s="3">
         <v>1.4999999999999999E-2</v>
       </c>
     </row>
@@ -5423,7 +5424,7 @@
       <c r="B14">
         <v>12</v>
       </c>
-      <c r="C14" s="4">
+      <c r="C14" s="3">
         <v>1.4E-2</v>
       </c>
     </row>
@@ -5434,7 +5435,7 @@
       <c r="B15">
         <v>2</v>
       </c>
-      <c r="C15" s="4">
+      <c r="C15" s="3">
         <v>2E-3</v>
       </c>
     </row>

</xml_diff>